<commit_message>
terminando o merge dos dados
</commit_message>
<xml_diff>
--- a/atletas.xlsx
+++ b/atletas.xlsx
@@ -41661,7 +41661,7 @@
       </c>
       <c r="B3172" t="inlineStr">
         <is>
-          <t>MARIELA MORAGA</t>
+          <t>HU XIAOYU, SHAN MENGYUAN</t>
         </is>
       </c>
       <c r="C3172" t="n">
@@ -41674,7 +41674,7 @@
       </c>
       <c r="B3173" t="inlineStr">
         <is>
-          <t>ELKAN RESHAWN OH</t>
+          <t>SAMANTHA EDWARDS</t>
         </is>
       </c>
       <c r="C3173" t="n">
@@ -41687,7 +41687,7 @@
       </c>
       <c r="B3174" t="inlineStr">
         <is>
-          <t>KENJI NANRI</t>
+          <t>FACUNDO OLEZZA</t>
         </is>
       </c>
       <c r="C3174" t="n">
@@ -41700,7 +41700,7 @@
       </c>
       <c r="B3175" t="inlineStr">
         <is>
-          <t>CAGLA DONERTAS</t>
+          <t>PAWEL TARNOWSKI</t>
         </is>
       </c>
       <c r="C3175" t="n">
@@ -41713,7 +41713,7 @@
       </c>
       <c r="B3176" t="inlineStr">
         <is>
-          <t>GABRIELLA KIDD</t>
+          <t>MARCELO CAIRO</t>
         </is>
       </c>
       <c r="C3176" t="n">
@@ -41726,7 +41726,7 @@
       </c>
       <c r="B3177" t="inlineStr">
         <is>
-          <t>MATISSE PACAUD, LUCIE GENNES</t>
+          <t>PAVLOS KONTIDES</t>
         </is>
       </c>
       <c r="C3177" t="n">
@@ -41739,7 +41739,7 @@
       </c>
       <c r="B3178" t="inlineStr">
         <is>
-          <t>HELENA WOLFF</t>
+          <t>NEIL MARCELLINI</t>
         </is>
       </c>
       <c r="C3178" t="n">
@@ -41752,7 +41752,7 @@
       </c>
       <c r="B3179" t="inlineStr">
         <is>
-          <t>PANAGIOTIS SPANOS</t>
+          <t>ALEKSI TAPPER</t>
         </is>
       </c>
       <c r="C3179" t="n">
@@ -41765,7 +41765,7 @@
       </c>
       <c r="B3180" t="inlineStr">
         <is>
-          <t>ATHANASIOS KYFIDIS</t>
+          <t>PATRICK SCALLY</t>
         </is>
       </c>
       <c r="C3180" t="n">
@@ -41778,7 +41778,7 @@
       </c>
       <c r="B3181" t="inlineStr">
         <is>
-          <t>DUKO BOS</t>
+          <t>ELI LIEFTING</t>
         </is>
       </c>
       <c r="C3181" t="n">
@@ -41791,7 +41791,7 @@
       </c>
       <c r="B3182" t="inlineStr">
         <is>
-          <t>MIRANDA PAPADAKI</t>
+          <t>VINCENT PETER</t>
         </is>
       </c>
       <c r="C3182" t="n">
@@ -41804,7 +41804,7 @@
       </c>
       <c r="B3183" t="inlineStr">
         <is>
-          <t>MILIVOJ DUKIC</t>
+          <t>SOFIIA NAUMENKO</t>
         </is>
       </c>
       <c r="C3183" t="n">
@@ -41817,7 +41817,7 @@
       </c>
       <c r="B3184" t="inlineStr">
         <is>
-          <t>YVES MERMOD, MAJA SIEGENTHALER</t>
+          <t>PEDRO FELIPE ROBLES, CARMINA SOFIA FUENTES</t>
         </is>
       </c>
       <c r="C3184" t="n">
@@ -41830,7 +41830,7 @@
       </c>
       <c r="B3185" t="inlineStr">
         <is>
-          <t>SAKAI AKIRA, AYLSWORTH RUSSELL</t>
+          <t>MAYA PILNIK</t>
         </is>
       </c>
       <c r="C3185" t="n">
@@ -41843,7 +41843,7 @@
       </c>
       <c r="B3186" t="inlineStr">
         <is>
-          <t>JOSEPHINE HEEGAARD</t>
+          <t>KATRINA MICALLEF</t>
         </is>
       </c>
       <c r="C3186" t="n">
@@ -41856,7 +41856,7 @@
       </c>
       <c r="B3187" t="inlineStr">
         <is>
-          <t>DUNCAN GREGOR, FREDDIE LONSDALE</t>
+          <t>BOZIDAR GOLUBIC</t>
         </is>
       </c>
       <c r="C3187" t="n">
@@ -41869,7 +41869,7 @@
       </c>
       <c r="B3188" t="inlineStr">
         <is>
-          <t>SHAI KAKON</t>
+          <t>ACHILLEAS GHICAS</t>
         </is>
       </c>
       <c r="C3188" t="n">
@@ -41882,7 +41882,7 @@
       </c>
       <c r="B3189" t="inlineStr">
         <is>
-          <t>GEORGIA LEWIN-LAFRANCE, ANTONIA LEWIN-LAFRANCE</t>
+          <t>PERNELLE MICHON</t>
         </is>
       </c>
       <c r="C3189" t="n">
@@ -41895,7 +41895,7 @@
       </c>
       <c r="B3190" t="inlineStr">
         <is>
-          <t>JOHAN SCHUBERT</t>
+          <t>JARROD JONES</t>
         </is>
       </c>
       <c r="C3190" t="n">
@@ -41908,7 +41908,7 @@
       </c>
       <c r="B3191" t="inlineStr">
         <is>
-          <t>MILLIE IRISH, SZYMON MATYJASZCZUK</t>
+          <t>MARSHA  BINTE SHAHRIN</t>
         </is>
       </c>
       <c r="C3191" t="n">
@@ -41921,7 +41921,7 @@
       </c>
       <c r="B3192" t="inlineStr">
         <is>
-          <t>JOANNA CYMERMAN, TYMON KOSOBUCKI</t>
+          <t>FILIP JURIIC</t>
         </is>
       </c>
       <c r="C3192" t="n">
@@ -41934,7 +41934,7 @@
       </c>
       <c r="B3193" t="inlineStr">
         <is>
-          <t>MAYA PILNIK</t>
+          <t>ZANGJUN XU, YIXIAO LYU</t>
         </is>
       </c>
       <c r="C3193" t="n">
@@ -41947,7 +41947,7 @@
       </c>
       <c r="B3194" t="inlineStr">
         <is>
-          <t>NICOLE VAN DER VELDEN VIZCAYA</t>
+          <t>TITOUAN  LE BOSQ</t>
         </is>
       </c>
       <c r="C3194" t="n">
@@ -41960,7 +41960,7 @@
       </c>
       <c r="B3195" t="inlineStr">
         <is>
-          <t>MATEUSZ GWOZDZ, LUKASZ MACHOWSKI</t>
+          <t>MAGGIE EILLEN PESCETTO</t>
         </is>
       </c>
       <c r="C3195" t="n">
@@ -41973,7 +41973,7 @@
       </c>
       <c r="B3196" t="inlineStr">
         <is>
-          <t>LUKE ELLIOTT</t>
+          <t>JAMES PERCIVAL</t>
         </is>
       </c>
       <c r="C3196" t="n">
@@ -41986,7 +41986,7 @@
       </c>
       <c r="B3197" t="inlineStr">
         <is>
-          <t>CONRAD KONITZER, ANTONIO TORRADO MARTINEZ</t>
+          <t>ALEXANDROS IOANNIDIS</t>
         </is>
       </c>
       <c r="C3197" t="n">
@@ -41999,7 +41999,7 @@
       </c>
       <c r="B3198" t="inlineStr">
         <is>
-          <t>MAELLE FRASCARI, SVEVA CARRARO</t>
+          <t>YUMIKO TOMBE</t>
         </is>
       </c>
       <c r="C3198" t="n">
@@ -42012,7 +42012,7 @@
       </c>
       <c r="B3199" t="inlineStr">
         <is>
-          <t>CAMILLE LECOINTRE, JEREMIE MION</t>
+          <t>MATISSE PACAUD, LUCIE GENNES</t>
         </is>
       </c>
       <c r="C3199" t="n">
@@ -42025,7 +42025,7 @@
       </c>
       <c r="B3200" t="inlineStr">
         <is>
-          <t>EMMA RENNIE</t>
+          <t>ILIJA MARKOVIC</t>
         </is>
       </c>
       <c r="C3200" t="n">
@@ -42038,7 +42038,7 @@
       </c>
       <c r="B3201" t="inlineStr">
         <is>
-          <t>VARVARA PORTOLOU</t>
+          <t>YUTA IRIE</t>
         </is>
       </c>
       <c r="C3201" t="n">
@@ -42051,7 +42051,7 @@
       </c>
       <c r="B3202" t="inlineStr">
         <is>
-          <t>KENJE SEM WERPERS</t>
+          <t>ESTERE KUMPINA</t>
         </is>
       </c>
       <c r="C3202" t="n">
@@ -42064,7 +42064,7 @@
       </c>
       <c r="B3203" t="inlineStr">
         <is>
-          <t>NITAI HASSON, NOA LASRY</t>
+          <t>GUSTAV AASHOLM-BRADLEY, FREDERIK RAGAN MELBYE</t>
         </is>
       </c>
       <c r="C3203" t="n">
@@ -42077,7 +42077,7 @@
       </c>
       <c r="B3204" t="inlineStr">
         <is>
-          <t>JAN PERNARCIC, GIOVANNI SANDRINI</t>
+          <t>SAMUEL DICKINSON</t>
         </is>
       </c>
       <c r="C3204" t="n">
@@ -42090,7 +42090,7 @@
       </c>
       <c r="B3205" t="inlineStr">
         <is>
-          <t>DYLAN FORSYTH</t>
+          <t>MAOR BENHAROCH</t>
         </is>
       </c>
       <c r="C3205" t="n">
@@ -42103,7 +42103,7 @@
       </c>
       <c r="B3206" t="inlineStr">
         <is>
-          <t>EMILE  ROULLET</t>
+          <t>ASCENSION ROCA DE TOGORES</t>
         </is>
       </c>
       <c r="C3206" t="n">
@@ -42116,7 +42116,7 @@
       </c>
       <c r="B3207" t="inlineStr">
         <is>
-          <t>VALADE LOMANE, JULIEN BUNEL</t>
+          <t>LOUKIANOS ZAMIT</t>
         </is>
       </c>
       <c r="C3207" t="n">
@@ -42129,7 +42129,7 @@
       </c>
       <c r="B3208" t="inlineStr">
         <is>
-          <t>SAMUEL DICKINSON</t>
+          <t>KRISTINA BOJA</t>
         </is>
       </c>
       <c r="C3208" t="n">
@@ -42142,7 +42142,7 @@
       </c>
       <c r="B3209" t="inlineStr">
         <is>
-          <t>JAMES PERCIVAL</t>
+          <t>FINN LYNCH</t>
         </is>
       </c>
       <c r="C3209" t="n">
@@ -42155,7 +42155,7 @@
       </c>
       <c r="B3210" t="inlineStr">
         <is>
-          <t>ROOS WIND</t>
+          <t>BENEDETTA SALLE, ALESSIO BELLICO</t>
         </is>
       </c>
       <c r="C3210" t="n">
@@ -42168,7 +42168,7 @@
       </c>
       <c r="B3211" t="inlineStr">
         <is>
-          <t>CRISTINA CASTELLANOS</t>
+          <t>KJELL HASCHEN, IVEN FROMM</t>
         </is>
       </c>
       <c r="C3211" t="n">
@@ -42181,7 +42181,7 @@
       </c>
       <c r="B3212" t="inlineStr">
         <is>
-          <t>ALESSANDRO FRACASSI</t>
+          <t>NITAI HASSON, NOA LASRY</t>
         </is>
       </c>
       <c r="C3212" t="n">
@@ -42194,7 +42194,7 @@
       </c>
       <c r="B3213" t="inlineStr">
         <is>
-          <t>TERUAKI SHIMAKURA, KAMISONODA SHINTARO SEIJI</t>
+          <t>MARTIN CLOOS, EMILIANA MARIA LOPEZ</t>
         </is>
       </c>
       <c r="C3213" t="n">
@@ -42207,7 +42207,7 @@
       </c>
       <c r="B3214" t="inlineStr">
         <is>
-          <t>DIMITRI PERONI</t>
+          <t>NETHRA KUMANAN</t>
         </is>
       </c>
       <c r="C3214" t="n">
@@ -42220,7 +42220,7 @@
       </c>
       <c r="B3215" t="inlineStr">
         <is>
-          <t>ACHILLEAS GHICAS</t>
+          <t>OTTO HENRY</t>
         </is>
       </c>
       <c r="C3215" t="n">
@@ -42233,7 +42233,7 @@
       </c>
       <c r="B3216" t="inlineStr">
         <is>
-          <t>ARISTOTELIS CHATZISTAMATIOU</t>
+          <t>CORENTIN GOULON, TIMOTHEE DEPERY</t>
         </is>
       </c>
       <c r="C3216" t="n">
@@ -42246,7 +42246,7 @@
       </c>
       <c r="B3217" t="inlineStr">
         <is>
-          <t>MILAN VUJASINOVIC</t>
+          <t>KENJE SEM WERPERS</t>
         </is>
       </c>
       <c r="C3217" t="n">
@@ -42259,7 +42259,7 @@
       </c>
       <c r="B3218" t="inlineStr">
         <is>
-          <t>WONN KYE LEE</t>
+          <t>KAREL RATNIK</t>
         </is>
       </c>
       <c r="C3218" t="n">
@@ -42272,7 +42272,7 @@
       </c>
       <c r="B3219" t="inlineStr">
         <is>
-          <t>ATHANASIOS TRIGKONIS</t>
+          <t>JOEL RODRIGUEZ PEREZ</t>
         </is>
       </c>
       <c r="C3219" t="n">
@@ -42285,7 +42285,7 @@
       </c>
       <c r="B3220" t="inlineStr">
         <is>
-          <t>ANNE MARIE RINDOM</t>
+          <t>ZACHEE WAYAG</t>
         </is>
       </c>
       <c r="C3220" t="n">
@@ -42298,7 +42298,7 @@
       </c>
       <c r="B3221" t="inlineStr">
         <is>
-          <t>MELINA PAPPA, NIKOLAS GIOTOPOULOS</t>
+          <t>SACHIN GANESH</t>
         </is>
       </c>
       <c r="C3221" t="n">
@@ -42311,7 +42311,7 @@
       </c>
       <c r="B3222" t="inlineStr">
         <is>
-          <t>CHRISTINA MARIA MENI</t>
+          <t>UMUT EYRIPARMAK</t>
         </is>
       </c>
       <c r="C3222" t="n">
@@ -42324,7 +42324,7 @@
       </c>
       <c r="B3223" t="inlineStr">
         <is>
-          <t>MIKHAIL NOVIKOV</t>
+          <t>MARU SCHEEL, FREYA FEILCKE</t>
         </is>
       </c>
       <c r="C3223" t="n">
@@ -42337,7 +42337,7 @@
       </c>
       <c r="B3224" t="inlineStr">
         <is>
-          <t>WEN ZAIDING, LIU TIAN</t>
+          <t>SAM KING</t>
         </is>
       </c>
       <c r="C3224" t="n">
@@ -42350,7 +42350,7 @@
       </c>
       <c r="B3225" t="inlineStr">
         <is>
-          <t>PARIS HENKEN, ANNA TOBIAS</t>
+          <t>CAMPBELL STANTON, WILL SHAPLAND</t>
         </is>
       </c>
       <c r="C3225" t="n">
@@ -42363,7 +42363,7 @@
       </c>
       <c r="B3226" t="inlineStr">
         <is>
-          <t>MARIJA ANDELA DE MICHELI-VITTURI, MIHAELA ZJENA DE MICHELI-VITTURI</t>
+          <t>ANTON MESSERITSCH</t>
         </is>
       </c>
       <c r="C3226" t="n">
@@ -42376,7 +42376,7 @@
       </c>
       <c r="B3227" t="inlineStr">
         <is>
-          <t>CLEMENS KUBBER</t>
+          <t>KENJI NANRI</t>
         </is>
       </c>
       <c r="C3227" t="n">
@@ -42389,7 +42389,7 @@
       </c>
       <c r="B3228" t="inlineStr">
         <is>
-          <t>ISAAC SCHOTTE</t>
+          <t>CHEN SHASHA, WANG MENGTING</t>
         </is>
       </c>
       <c r="C3228" t="n">
@@ -42402,7 +42402,7 @@
       </c>
       <c r="B3229" t="inlineStr">
         <is>
-          <t>MANON PEYRE CLARA-SOFIA, STAMMINGER DE MOURA</t>
+          <t>ANDREW VERDYSH</t>
         </is>
       </c>
       <c r="C3229" t="n">
@@ -42415,7 +42415,7 @@
       </c>
       <c r="B3230" t="inlineStr">
         <is>
-          <t>NEUS BALLESTER, CARLOTA GARCIA</t>
+          <t>JULIA BUSSELBERG</t>
         </is>
       </c>
       <c r="C3230" t="n">
@@ -42428,7 +42428,7 @@
       </c>
       <c r="B3231" t="inlineStr">
         <is>
-          <t>JULIA BUSSELBERG</t>
+          <t>YIGIT YALCIN CITAK</t>
         </is>
       </c>
       <c r="C3231" t="n">
@@ -42441,7 +42441,7 @@
       </c>
       <c r="B3232" t="inlineStr">
         <is>
-          <t>CATALINA TURIENZO</t>
+          <t>PETRA MASTELIC</t>
         </is>
       </c>
       <c r="C3232" t="n">
@@ -42454,7 +42454,7 @@
       </c>
       <c r="B3233" t="inlineStr">
         <is>
-          <t>NEIL MARCELLINI</t>
+          <t>GIACOMO FERRARI, ALESSANDRA DUBBINI</t>
         </is>
       </c>
       <c r="C3233" t="n">
@@ -42467,7 +42467,7 @@
       </c>
       <c r="B3234" t="inlineStr">
         <is>
-          <t>ANDREW VERDYSH</t>
+          <t>ALESSANDRO FRACASSI</t>
         </is>
       </c>
       <c r="C3234" t="n">
@@ -42480,7 +42480,7 @@
       </c>
       <c r="B3235" t="inlineStr">
         <is>
-          <t>IAKOVOS CHRISTOFIDIS</t>
+          <t>SANTIAGO SAMPAIO</t>
         </is>
       </c>
       <c r="C3235" t="n">
@@ -42493,7 +42493,7 @@
       </c>
       <c r="B3236" t="inlineStr">
         <is>
-          <t>MARIA JOSE PONCEL MAURIN</t>
+          <t>JOSH MORGAN</t>
         </is>
       </c>
       <c r="C3236" t="n">
@@ -42506,7 +42506,7 @@
       </c>
       <c r="B3237" t="inlineStr">
         <is>
-          <t>CATERINA ROMERO</t>
+          <t>RINA  NIIJIMA</t>
         </is>
       </c>
       <c r="C3237" t="n">
@@ -42519,7 +42519,7 @@
       </c>
       <c r="B3238" t="inlineStr">
         <is>
-          <t>NITIPHAT    CHAIWUTTIWET</t>
+          <t>CRISTINA CASTELLANOS</t>
         </is>
       </c>
       <c r="C3238" t="n">
@@ -42532,7 +42532,7 @@
       </c>
       <c r="B3239" t="inlineStr">
         <is>
-          <t>KENNETH FREDERIKSEN</t>
+          <t>FILLAH KARIM</t>
         </is>
       </c>
       <c r="C3239" t="n">
@@ -42545,7 +42545,7 @@
       </c>
       <c r="B3240" t="inlineStr">
         <is>
-          <t>DAVID SURKOV</t>
+          <t>YELYZAVETA VYNOHRADOVA</t>
         </is>
       </c>
       <c r="C3240" t="n">
@@ -42558,7 +42558,7 @@
       </c>
       <c r="B3241" t="inlineStr">
         <is>
-          <t>NIKOLA BANJAC</t>
+          <t>MIHAIL BERBEROV</t>
         </is>
       </c>
       <c r="C3241" t="n">
@@ -42571,7 +42571,7 @@
       </c>
       <c r="B3242" t="inlineStr">
         <is>
-          <t>LACHIE WEBER</t>
+          <t>LUCIANA CARDOZO</t>
         </is>
       </c>
       <c r="C3242" t="n">
@@ -42584,7 +42584,7 @@
       </c>
       <c r="B3243" t="inlineStr">
         <is>
-          <t>PAUL  NAPOLEONE</t>
+          <t>WUNIU AYU</t>
         </is>
       </c>
       <c r="C3243" t="n">
@@ -42597,7 +42597,7 @@
       </c>
       <c r="B3244" t="inlineStr">
         <is>
-          <t>CHARLIE LEIGH, RYAN ORR</t>
+          <t>PERINE MILLERET</t>
         </is>
       </c>
       <c r="C3244" t="n">
@@ -42610,7 +42610,7 @@
       </c>
       <c r="B3245" t="inlineStr">
         <is>
-          <t>MANASE ICHIHASHI, RINKO GOTO</t>
+          <t>CASEY IMENEO</t>
         </is>
       </c>
       <c r="C3245" t="n">
@@ -42623,7 +42623,7 @@
       </c>
       <c r="B3246" t="inlineStr">
         <is>
-          <t>BEATA DOKOUPILOVA</t>
+          <t>B  LINDSAY</t>
         </is>
       </c>
       <c r="C3246" t="n">
@@ -42636,7 +42636,7 @@
       </c>
       <c r="B3247" t="inlineStr">
         <is>
-          <t>MARGA PERELLO</t>
+          <t>ELISAVET ILIOPOULOU</t>
         </is>
       </c>
       <c r="C3247" t="n">
@@ -42649,7 +42649,7 @@
       </c>
       <c r="B3248" t="inlineStr">
         <is>
-          <t>RADVILAS JANULIONIS</t>
+          <t>NICHOLAS HALLIDAY</t>
         </is>
       </c>
       <c r="C3248" t="n">
@@ -42662,7 +42662,7 @@
       </c>
       <c r="B3249" t="inlineStr">
         <is>
-          <t>KARL MARTIN RAMMO</t>
+          <t>CLEMENS KUBBER</t>
         </is>
       </c>
       <c r="C3249" t="n">
@@ -42675,7 +42675,7 @@
       </c>
       <c r="B3250" t="inlineStr">
         <is>
-          <t>FERDINAND STEFFAN</t>
+          <t>MILIVOJ DUKIC</t>
         </is>
       </c>
       <c r="C3250" t="n">
@@ -42688,7 +42688,7 @@
       </c>
       <c r="B3251" t="inlineStr">
         <is>
-          <t>PHILIPPE ETTORE</t>
+          <t>JOHN GORDON</t>
         </is>
       </c>
       <c r="C3251" t="n">
@@ -42701,7 +42701,7 @@
       </c>
       <c r="B3252" t="inlineStr">
         <is>
-          <t>GIORGIA DELLA VALLE</t>
+          <t>ANDRIANI GEORGIOU</t>
         </is>
       </c>
       <c r="C3252" t="n">
@@ -42714,7 +42714,7 @@
       </c>
       <c r="B3253" t="inlineStr">
         <is>
-          <t>NIKOLA  GIRKE</t>
+          <t>SARA SZENTIVANYI</t>
         </is>
       </c>
       <c r="C3253" t="n">
@@ -42727,7 +42727,7 @@
       </c>
       <c r="B3254" t="inlineStr">
         <is>
-          <t>LAMPROS NIKOLAOS GARMPIS</t>
+          <t>NELL DE ZAHAM</t>
         </is>
       </c>
       <c r="C3254" t="n">
@@ -42740,7 +42740,7 @@
       </c>
       <c r="B3255" t="inlineStr">
         <is>
-          <t>SAKI MATSUNAE, ERI HATAYAMA</t>
+          <t>STIPE GASPIC</t>
         </is>
       </c>
       <c r="C3255" t="n">
@@ -42753,7 +42753,7 @@
       </c>
       <c r="B3256" t="inlineStr">
         <is>
-          <t>BENEDETTA SALLE, ALESSIO BELLICO</t>
+          <t>ILIJA MARKOVIAE</t>
         </is>
       </c>
       <c r="C3256" t="n">
@@ -42766,7 +42766,7 @@
       </c>
       <c r="B3257" t="inlineStr">
         <is>
-          <t>TOMMASO BOCCUNI</t>
+          <t>FINLEY DICKINSON</t>
         </is>
       </c>
       <c r="C3257" t="n">
@@ -42779,7 +42779,7 @@
       </c>
       <c r="B3258" t="inlineStr">
         <is>
-          <t>MARTIN CLOOS, EMILIANA MARIA LOPEZ</t>
+          <t>CHIARA  FERRETTI</t>
         </is>
       </c>
       <c r="C3258" t="n">
@@ -42792,7 +42792,7 @@
       </c>
       <c r="B3259" t="inlineStr">
         <is>
-          <t>TRISTEN ERIK  KIVI</t>
+          <t>REBECCA MANTEL</t>
         </is>
       </c>
       <c r="C3259" t="n">
@@ -42805,7 +42805,7 @@
       </c>
       <c r="B3260" t="inlineStr">
         <is>
-          <t>ARGYRO KOURAVELOU</t>
+          <t>CRISTINA PUJOL BAJO</t>
         </is>
       </c>
       <c r="C3260" t="n">
@@ -42818,7 +42818,7 @@
       </c>
       <c r="B3261" t="inlineStr">
         <is>
-          <t>YULONG QIU</t>
+          <t>CARLOTTA RIZZARDI</t>
         </is>
       </c>
       <c r="C3261" t="n">
@@ -42831,7 +42831,7 @@
       </c>
       <c r="B3262" t="inlineStr">
         <is>
-          <t>BOZIDAR GOLUBIC</t>
+          <t>MARIELA MORAGA</t>
         </is>
       </c>
       <c r="C3262" t="n">
@@ -42844,7 +42844,7 @@
       </c>
       <c r="B3263" t="inlineStr">
         <is>
-          <t>MAKOTO TOMIZAWA</t>
+          <t>WILHELM KARK</t>
         </is>
       </c>
       <c r="C3263" t="n">
@@ -42857,7 +42857,7 @@
       </c>
       <c r="B3264" t="inlineStr">
         <is>
-          <t>ASCENSION ROCA DE TOGORES BENABENT</t>
+          <t>JULIA GOMEZ ROA</t>
         </is>
       </c>
       <c r="C3264" t="n">
@@ -42870,7 +42870,7 @@
       </c>
       <c r="B3265" t="inlineStr">
         <is>
-          <t>OKYANUS ARIKAN</t>
+          <t>ATHANASIOS KYFIDIS</t>
         </is>
       </c>
       <c r="C3265" t="n">
@@ -42883,7 +42883,7 @@
       </c>
       <c r="B3266" t="inlineStr">
         <is>
-          <t>NICO PARLIER</t>
+          <t>MARGA PERELLO</t>
         </is>
       </c>
       <c r="C3266" t="n">
@@ -42896,7 +42896,7 @@
       </c>
       <c r="B3267" t="inlineStr">
         <is>
-          <t>TIMO COUPEK</t>
+          <t>MALTHE EBDRUP, CLEMENT AASHOLM-BRADLEY</t>
         </is>
       </c>
       <c r="C3267" t="n">
@@ -42909,7 +42909,7 @@
       </c>
       <c r="B3268" t="inlineStr">
         <is>
-          <t>CHIARA  FERRETTI</t>
+          <t>GUILHERME  PLENTZ</t>
         </is>
       </c>
       <c r="C3268" t="n">
@@ -42922,7 +42922,7 @@
       </c>
       <c r="B3269" t="inlineStr">
         <is>
-          <t>SHINGEN FURUYA, AKIRA TAKAYANAGI</t>
+          <t>GUSTAVO ABDULKLECH, NICOLAS BERNAL</t>
         </is>
       </c>
       <c r="C3269" t="n">
@@ -42935,7 +42935,7 @@
       </c>
       <c r="B3270" t="inlineStr">
         <is>
-          <t>MARLA BERGMANN, HANNA WILLE</t>
+          <t>MICHAL MAZIARKA</t>
         </is>
       </c>
       <c r="C3270" t="n">
@@ -42948,7 +42948,7 @@
       </c>
       <c r="B3271" t="inlineStr">
         <is>
-          <t>JAMES QUENTIN BURNS</t>
+          <t>CATALINA TURIENZO</t>
         </is>
       </c>
       <c r="C3271" t="n">
@@ -42961,7 +42961,7 @@
       </c>
       <c r="B3272" t="inlineStr">
         <is>
-          <t>ISHWARIYA GANESH</t>
+          <t>DENISE HELENA RUI PARRUQUE, ALCIDIO PORTUGAL ALMEIDA LINO</t>
         </is>
       </c>
       <c r="C3272" t="n">
@@ -42974,7 +42974,7 @@
       </c>
       <c r="B3273" t="inlineStr">
         <is>
-          <t>BRUNO GASPIC</t>
+          <t>DILARA URALP PALOMBO</t>
         </is>
       </c>
       <c r="C3273" t="n">
@@ -42987,7 +42987,7 @@
       </c>
       <c r="B3274" t="inlineStr">
         <is>
-          <t>ESTERE KUMPINA</t>
+          <t>MARIA LILI ZAMIT</t>
         </is>
       </c>
       <c r="C3274" t="n">
@@ -43000,7 +43000,7 @@
       </c>
       <c r="B3275" t="inlineStr">
         <is>
-          <t>NUR SHAZRIN MOHAMAD LATIF</t>
+          <t>WEN ZAIDING, LIU TIAN</t>
         </is>
       </c>
       <c r="C3275" t="n">
@@ -43013,7 +43013,7 @@
       </c>
       <c r="B3276" t="inlineStr">
         <is>
-          <t>JOEL RODRIGUEZ PEREZ</t>
+          <t>ANATOL SASSI</t>
         </is>
       </c>
       <c r="C3276" t="n">
@@ -43026,7 +43026,7 @@
       </c>
       <c r="B3277" t="inlineStr">
         <is>
-          <t>ANGELO SOLI</t>
+          <t>ZOFIA KORSAK, MIKOLAJ BAZYLI</t>
         </is>
       </c>
       <c r="C3277" t="n">
@@ -43039,7 +43039,7 @@
       </c>
       <c r="B3278" t="inlineStr">
         <is>
-          <t>FUJIKO ONISHI</t>
+          <t>ATHANASIOS TRIGKONIS</t>
         </is>
       </c>
       <c r="C3278" t="n">
@@ -43052,7 +43052,7 @@
       </c>
       <c r="B3279" t="inlineStr">
         <is>
-          <t>DILARA URALP PALOMBO</t>
+          <t>EMMA RENNIE</t>
         </is>
       </c>
       <c r="C3279" t="n">
@@ -43065,7 +43065,7 @@
       </c>
       <c r="B3280" t="inlineStr">
         <is>
-          <t>MYKHAILO BILOHORODSKYI, POLINA ZATOCHNA</t>
+          <t>NUR SHAZRIN MOHAMAD LATIF</t>
         </is>
       </c>
       <c r="C3280" t="n">
@@ -43078,7 +43078,7 @@
       </c>
       <c r="B3281" t="inlineStr">
         <is>
-          <t>LIAM BRUCE</t>
+          <t>PAUL  NAPOLEONE</t>
         </is>
       </c>
       <c r="C3281" t="n">
@@ -43091,7 +43091,7 @@
       </c>
       <c r="B3282" t="inlineStr">
         <is>
-          <t>MIRTHE AKKERMAN</t>
+          <t>DIEGO BOTIN FLORIAN, TRITTEL PAUL</t>
         </is>
       </c>
       <c r="C3282" t="n">
@@ -43104,7 +43104,7 @@
       </c>
       <c r="B3283" t="inlineStr">
         <is>
-          <t>HERMANN TOMASGAARD</t>
+          <t>TATIANI BOUGIATIOTI</t>
         </is>
       </c>
       <c r="C3283" t="n">
@@ -43117,7 +43117,7 @@
       </c>
       <c r="B3284" t="inlineStr">
         <is>
-          <t>PAULA VAN WIERINGEN MASSANET, CLAUDIA SOBRAL LUSQUINOS</t>
+          <t>ALEXANDER BIJKERK</t>
         </is>
       </c>
       <c r="C3284" t="n">
@@ -43130,7 +43130,7 @@
       </c>
       <c r="B3285" t="inlineStr">
         <is>
-          <t>ANDREA TORRES FULLANA</t>
+          <t>URSULA BALAS</t>
         </is>
       </c>
       <c r="C3285" t="n">
@@ -43143,7 +43143,7 @@
       </c>
       <c r="B3286" t="inlineStr">
         <is>
-          <t>PERINE MILLERET</t>
+          <t>MIA MARIN LILIENTHAL</t>
         </is>
       </c>
       <c r="C3286" t="n">
@@ -43156,7 +43156,7 @@
       </c>
       <c r="B3287" t="inlineStr">
         <is>
-          <t>IAN BARROWS, HANS HENKEN</t>
+          <t>SAMUEL ABEN</t>
         </is>
       </c>
       <c r="C3287" t="n">
@@ -43169,7 +43169,7 @@
       </c>
       <c r="B3288" t="inlineStr">
         <is>
-          <t>KENNETH FREDERIKSEN FREDERIKSEN</t>
+          <t>ANTUN TOMASEVIC</t>
         </is>
       </c>
       <c r="C3288" t="n">
@@ -43182,7 +43182,7 @@
       </c>
       <c r="B3289" t="inlineStr">
         <is>
-          <t>CRISTINA PUJOL BAJO</t>
+          <t>ELISA HARTENBERGER</t>
         </is>
       </c>
       <c r="C3289" t="n">
@@ -43195,7 +43195,7 @@
       </c>
       <c r="B3290" t="inlineStr">
         <is>
-          <t>YANNICK LEFEBVRE, YOUENN BERTIN</t>
+          <t>DANIEL COSTANDI</t>
         </is>
       </c>
       <c r="C3290" t="n">
@@ -43208,7 +43208,7 @@
       </c>
       <c r="B3291" t="inlineStr">
         <is>
-          <t>JAGO HUERCANOS MACHIMBARRENA</t>
+          <t>ROOS WIND</t>
         </is>
       </c>
       <c r="C3291" t="n">
@@ -43221,7 +43221,7 @@
       </c>
       <c r="B3292" t="inlineStr">
         <is>
-          <t>B  LINDSAY</t>
+          <t>MARIA JOSE CUCALON, JONATHAN MARTINETTI</t>
         </is>
       </c>
       <c r="C3292" t="n">
@@ -43234,7 +43234,7 @@
       </c>
       <c r="B3293" t="inlineStr">
         <is>
-          <t>CHARLOTTE VIDELO</t>
+          <t>ARIE MOFFAT, HUNTER HOY</t>
         </is>
       </c>
       <c r="C3293" t="n">
@@ -43247,7 +43247,7 @@
       </c>
       <c r="B3294" t="inlineStr">
         <is>
-          <t>LUCY BILGER</t>
+          <t>ALFONSO FERNANDEZ</t>
         </is>
       </c>
       <c r="C3294" t="n">
@@ -43260,7 +43260,7 @@
       </c>
       <c r="B3295" t="inlineStr">
         <is>
-          <t>JOSEPH JONATHAN PEN WESTON</t>
+          <t>JOANNA CYMERMAN, TYMON KOSOBUCKI</t>
         </is>
       </c>
       <c r="C3295" t="n">
@@ -43273,7 +43273,7 @@
       </c>
       <c r="B3296" t="inlineStr">
         <is>
-          <t>MARSHA  BINTE SHAHRIN</t>
+          <t>MILAN VUJASINOVIC</t>
         </is>
       </c>
       <c r="C3296" t="n">
@@ -43286,7 +43286,7 @@
       </c>
       <c r="B3297" t="inlineStr">
         <is>
-          <t>PAVLOS KONTIDES</t>
+          <t>ELYSE AINSWORTH</t>
         </is>
       </c>
       <c r="C3297" t="n">
@@ -43299,7 +43299,7 @@
       </c>
       <c r="B3298" t="inlineStr">
         <is>
-          <t>MARIT BOUWMEESTER</t>
+          <t>FERDINAND STEFFAN</t>
         </is>
       </c>
       <c r="C3298" t="n">
@@ -43312,7 +43312,7 @@
       </c>
       <c r="B3299" t="inlineStr">
         <is>
-          <t>OMER VERED VILENCHIK</t>
+          <t>YOGEV ALCALAY</t>
         </is>
       </c>
       <c r="C3299" t="n">
@@ -43325,7 +43325,7 @@
       </c>
       <c r="B3300" t="inlineStr">
         <is>
-          <t>JAMES PETERS, FYNN STERRITT</t>
+          <t>TOMMASO BOCCUNI</t>
         </is>
       </c>
       <c r="C3300" t="n">
@@ -43338,7 +43338,7 @@
       </c>
       <c r="B3301" t="inlineStr">
         <is>
-          <t>THEO REVIL, YANN JAUVIN</t>
+          <t>CATERINA ROMERO</t>
         </is>
       </c>
       <c r="C3301" t="n">
@@ -43351,7 +43351,7 @@
       </c>
       <c r="B3302" t="inlineStr">
         <is>
-          <t>ALEXANDER BIJKERK</t>
+          <t>ARGYRO KOURAVELOU</t>
         </is>
       </c>
       <c r="C3302" t="n">
@@ -43364,7 +43364,7 @@
       </c>
       <c r="B3303" t="inlineStr">
         <is>
-          <t>HONOKA MIURA</t>
+          <t>PIA CONRADI</t>
         </is>
       </c>
       <c r="C3303" t="n">
@@ -43377,7 +43377,7 @@
       </c>
       <c r="B3304" t="inlineStr">
         <is>
-          <t>FILIP OLSZEWSKI</t>
+          <t>DUNCAN GREGOR, FREDDIE LONSDALE</t>
         </is>
       </c>
       <c r="C3304" t="n">
@@ -43390,7 +43390,7 @@
       </c>
       <c r="B3305" t="inlineStr">
         <is>
-          <t>REBECCA MANTEL</t>
+          <t>UFFE TOMASGAARD</t>
         </is>
       </c>
       <c r="C3305" t="n">
@@ -43403,7 +43403,7 @@
       </c>
       <c r="B3306" t="inlineStr">
         <is>
-          <t>MOHIT SAINI</t>
+          <t>JAMES PETERS, FYNN STERRITT</t>
         </is>
       </c>
       <c r="C3306" t="n">
@@ -43416,7 +43416,7 @@
       </c>
       <c r="B3307" t="inlineStr">
         <is>
-          <t>NELL DE ZAHAM</t>
+          <t>MICHAEL LEIGH</t>
         </is>
       </c>
       <c r="C3307" t="n">
@@ -43429,7 +43429,7 @@
       </c>
       <c r="B3308" t="inlineStr">
         <is>
-          <t>CARLOS ESPI</t>
+          <t>SAMUEL OLIVER SILLS</t>
         </is>
       </c>
       <c r="C3308" t="n">
@@ -43442,7 +43442,7 @@
       </c>
       <c r="B3309" t="inlineStr">
         <is>
-          <t>NICOL SEGNINI</t>
+          <t>FORD MCCANN</t>
         </is>
       </c>
       <c r="C3309" t="n">
@@ -43455,7 +43455,7 @@
       </c>
       <c r="B3310" t="inlineStr">
         <is>
-          <t>ASCENSION ROCA DE TOGORES</t>
+          <t>MATILDA TALLURI</t>
         </is>
       </c>
       <c r="C3310" t="n">
@@ -43468,7 +43468,7 @@
       </c>
       <c r="B3311" t="inlineStr">
         <is>
-          <t>FERRUCCIO ARVEDI</t>
+          <t>ROBBY MEEK</t>
         </is>
       </c>
       <c r="C3311" t="n">
@@ -43481,7 +43481,7 @@
       </c>
       <c r="B3312" t="inlineStr">
         <is>
-          <t>URSULA BALAS</t>
+          <t>BEN FLOWER</t>
         </is>
       </c>
       <c r="C3312" t="n">
@@ -43494,7 +43494,7 @@
       </c>
       <c r="B3313" t="inlineStr">
         <is>
-          <t>MIA MARIN LILIENTHAL</t>
+          <t>LINE FLEM HOEST</t>
         </is>
       </c>
       <c r="C3313" t="n">
@@ -43507,7 +43507,7 @@
       </c>
       <c r="B3314" t="inlineStr">
         <is>
-          <t>ZANGJUN XU, YIXIAO LYU</t>
+          <t>MANASE ICHIHASHI, RINKO GOTO</t>
         </is>
       </c>
       <c r="C3314" t="n">
@@ -43520,7 +43520,7 @@
       </c>
       <c r="B3315" t="inlineStr">
         <is>
-          <t>ZOFIA KORSAK, MIKOLAJ BAZYLI</t>
+          <t>VYRON KOKKALANIS</t>
         </is>
       </c>
       <c r="C3315" t="n">
@@ -43533,7 +43533,7 @@
       </c>
       <c r="B3316" t="inlineStr">
         <is>
-          <t>PATRICK SCALLY</t>
+          <t>WONN KYE LEE</t>
         </is>
       </c>
       <c r="C3316" t="n">
@@ -43546,7 +43546,7 @@
       </c>
       <c r="B3317" t="inlineStr">
         <is>
-          <t>HONG WEI, LV HONGMING</t>
+          <t>MICHAEL PALIOS</t>
         </is>
       </c>
       <c r="C3317" t="n">
@@ -43559,7 +43559,7 @@
       </c>
       <c r="B3318" t="inlineStr">
         <is>
-          <t>JUAN MAEGLI</t>
+          <t>HERNAN UMPIERRE, FERNANDO DIZ</t>
         </is>
       </c>
       <c r="C3318" t="n">
@@ -43572,7 +43572,7 @@
       </c>
       <c r="B3319" t="inlineStr">
         <is>
-          <t>MARIA LILI ZAMIT</t>
+          <t>OSKAR MADONICH</t>
         </is>
       </c>
       <c r="C3319" t="n">
@@ -43585,7 +43585,7 @@
       </c>
       <c r="B3320" t="inlineStr">
         <is>
-          <t>JORDI XAMMAR, NORA BRUGMAN</t>
+          <t>PEP CAZADOR</t>
         </is>
       </c>
       <c r="C3320" t="n">
@@ -43598,7 +43598,7 @@
       </c>
       <c r="B3321" t="inlineStr">
         <is>
-          <t>JULIA GOMEZ ROA</t>
+          <t>VARVARA PORTOLOU</t>
         </is>
       </c>
       <c r="C3321" t="n">
@@ -43611,7 +43611,7 @@
       </c>
       <c r="B3322" t="inlineStr">
         <is>
-          <t>BARBARA WINAU ORDINAS</t>
+          <t>MAELLE FRASCARI, SVEVA CARRARO</t>
         </is>
       </c>
       <c r="C3322" t="n">
@@ -43624,7 +43624,7 @@
       </c>
       <c r="B3323" t="inlineStr">
         <is>
-          <t>ANDREAS KRABBE CHRISTENSEN</t>
+          <t>GEORGIA LEWIN-LAFRANCE, ANTONIA LEWIN-LAFRANCE</t>
         </is>
       </c>
       <c r="C3323" t="n">
@@ -43637,7 +43637,7 @@
       </c>
       <c r="B3324" t="inlineStr">
         <is>
-          <t>DIMITRIOS ANASTASIADIS</t>
+          <t>PHILIPPE ETTORE</t>
         </is>
       </c>
       <c r="C3324" t="n">
@@ -43650,7 +43650,7 @@
       </c>
       <c r="B3325" t="inlineStr">
         <is>
-          <t>SHEILA MARTINEZ</t>
+          <t>MAOR BEN HAROSH</t>
         </is>
       </c>
       <c r="C3325" t="n">
@@ -43663,7 +43663,7 @@
       </c>
       <c r="B3326" t="inlineStr">
         <is>
-          <t>AI YOSHIDA, YUGO YOSHIDA</t>
+          <t>MIKHAIL NOVIKOV</t>
         </is>
       </c>
       <c r="C3326" t="n">
@@ -43676,7 +43676,7 @@
       </c>
       <c r="B3327" t="inlineStr">
         <is>
-          <t>ATTILIO BORIO</t>
+          <t>TOMASZ BENDLEWSKI</t>
         </is>
       </c>
       <c r="C3327" t="n">
@@ -43689,7 +43689,7 @@
       </c>
       <c r="B3328" t="inlineStr">
         <is>
-          <t>DIONISIS FATSIADIS</t>
+          <t>JAKOB MEGGENDORFER, ANDREAS SPRANGER</t>
         </is>
       </c>
       <c r="C3328" t="n">
@@ -43702,7 +43702,7 @@
       </c>
       <c r="B3329" t="inlineStr">
         <is>
-          <t>KACPER PASZEK, IGA WIELCZYK</t>
+          <t>MARIA SOL BRANZ CRESPO, JULIA PANTIN</t>
         </is>
       </c>
       <c r="C3329" t="n">
@@ -43715,7 +43715,7 @@
       </c>
       <c r="B3330" t="inlineStr">
         <is>
-          <t>SANTIAGO SAMPAIO</t>
+          <t>ENRICHETTA BETTINI FLEITAS</t>
         </is>
       </c>
       <c r="C3330" t="n">
@@ -43728,7 +43728,7 @@
       </c>
       <c r="B3331" t="inlineStr">
         <is>
-          <t>MAGGIE EILLEN PESCETTO</t>
+          <t>ARISTOTELIS CHATZISTAMATIOU</t>
         </is>
       </c>
       <c r="C3331" t="n">
@@ -43741,7 +43741,7 @@
       </c>
       <c r="B3332" t="inlineStr">
         <is>
-          <t>TAEHOON LEE</t>
+          <t>MANON PEYRE CLARA-SOFIA, STAMMINGER DE MOURA</t>
         </is>
       </c>
       <c r="C3332" t="n">
@@ -43754,7 +43754,7 @@
       </c>
       <c r="B3333" t="inlineStr">
         <is>
-          <t>HERMIONIE GHICAS</t>
+          <t>ANA MONCADA</t>
         </is>
       </c>
       <c r="C3333" t="n">
@@ -43767,7 +43767,7 @@
       </c>
       <c r="B3334" t="inlineStr">
         <is>
-          <t>WANG YINGQIAN, XIAOYA SU</t>
+          <t>TIM</t>
         </is>
       </c>
       <c r="C3334" t="n">
@@ -43780,7 +43780,7 @@
       </c>
       <c r="B3335" t="inlineStr">
         <is>
-          <t>STANISLAW  TREPCZYNSKI</t>
+          <t>LACHIE WEBER</t>
         </is>
       </c>
       <c r="C3335" t="n">
@@ -43793,7 +43793,7 @@
       </c>
       <c r="B3336" t="inlineStr">
         <is>
-          <t>KIKO PEIRO</t>
+          <t>KENNETH FREDERIKSEN FREDERIKSEN</t>
         </is>
       </c>
       <c r="C3336" t="n">
@@ -43806,7 +43806,7 @@
       </c>
       <c r="B3337" t="inlineStr">
         <is>
-          <t>ANDRIANI GEORGIOU</t>
+          <t>ERWAN FISCHER, CLEMENT PEQUIN</t>
         </is>
       </c>
       <c r="C3337" t="n">
@@ -43819,7 +43819,7 @@
       </c>
       <c r="B3338" t="inlineStr">
         <is>
-          <t>CHEN SHASHA, WANG MENGTING</t>
+          <t>ANDREA TORRES FULLANA</t>
         </is>
       </c>
       <c r="C3338" t="n">
@@ -43832,7 +43832,7 @@
       </c>
       <c r="B3339" t="inlineStr">
         <is>
-          <t>JAMES GRUMMETT, RHOS HAWES</t>
+          <t>HAMISH GILSENAN</t>
         </is>
       </c>
       <c r="C3339" t="n">
@@ -43845,7 +43845,7 @@
       </c>
       <c r="B3340" t="inlineStr">
         <is>
-          <t>MICHAL MAZIARKA</t>
+          <t>MAKOTO TOMIZAWA</t>
         </is>
       </c>
       <c r="C3340" t="n">
@@ -43858,7 +43858,7 @@
       </c>
       <c r="B3341" t="inlineStr">
         <is>
-          <t>INGA-MARIE HOFMANN, CATHERINE BARTELHEIMER</t>
+          <t>ENRICO TANFERNA</t>
         </is>
       </c>
       <c r="C3341" t="n">
@@ -43871,7 +43871,7 @@
       </c>
       <c r="B3342" t="inlineStr">
         <is>
-          <t>WILHELM KARK</t>
+          <t>IAN BARROWS, HANS HENKEN</t>
         </is>
       </c>
       <c r="C3342" t="n">
@@ -43884,7 +43884,7 @@
       </c>
       <c r="B3343" t="inlineStr">
         <is>
-          <t>ALISE SANTORUM</t>
+          <t>JOHAN SCHUBERT</t>
         </is>
       </c>
       <c r="C3343" t="n">
@@ -43897,7 +43897,7 @@
       </c>
       <c r="B3344" t="inlineStr">
         <is>
-          <t>OSKAR MADONICH</t>
+          <t>WILLEM WIERSEMA</t>
         </is>
       </c>
       <c r="C3344" t="n">
@@ -43910,7 +43910,7 @@
       </c>
       <c r="B3345" t="inlineStr">
         <is>
-          <t>CHRIS BOBOTAS</t>
+          <t>EDWARD REID</t>
         </is>
       </c>
       <c r="C3345" t="n">
@@ -43923,7 +43923,7 @@
       </c>
       <c r="B3346" t="inlineStr">
         <is>
-          <t>NICHOLAS HALLIDAY</t>
+          <t>LENNART KUSS</t>
         </is>
       </c>
       <c r="C3346" t="n">
@@ -43936,7 +43936,7 @@
       </c>
       <c r="B3347" t="inlineStr">
         <is>
-          <t>UMUT EYRIPARMAK</t>
+          <t>JONAH MAIER</t>
         </is>
       </c>
       <c r="C3347" t="n">
@@ -43949,7 +43949,7 @@
       </c>
       <c r="B3348" t="inlineStr">
         <is>
-          <t>PAOLO FREDDI</t>
+          <t>CAGLA DONERTAS</t>
         </is>
       </c>
       <c r="C3348" t="n">
@@ -43962,7 +43962,7 @@
       </c>
       <c r="B3349" t="inlineStr">
         <is>
-          <t>MARU SCHEEL, FREYA FEILCKE</t>
+          <t>DIONISIS FATSIADIS</t>
         </is>
       </c>
       <c r="C3349" t="n">
@@ -43975,7 +43975,7 @@
       </c>
       <c r="B3350" t="inlineStr">
         <is>
-          <t>SEBASTIEN SCHNEITER, ARNO DE PLANTA</t>
+          <t>MEGUMI ISEDA</t>
         </is>
       </c>
       <c r="C3350" t="n">
@@ -43988,7 +43988,7 @@
       </c>
       <c r="B3351" t="inlineStr">
         <is>
-          <t>ALEKSI TAPPER</t>
+          <t>TOM HOLMES</t>
         </is>
       </c>
       <c r="C3351" t="n">
@@ -44001,7 +44001,7 @@
       </c>
       <c r="B3352" t="inlineStr">
         <is>
-          <t>TITOUAN  LE BOSQ</t>
+          <t>HONG WEI, LV HONGMING</t>
         </is>
       </c>
       <c r="C3352" t="n">
@@ -44014,7 +44014,7 @@
       </c>
       <c r="B3353" t="inlineStr">
         <is>
-          <t>JONAH MAIER</t>
+          <t>ALENKA VALENCIC</t>
         </is>
       </c>
       <c r="C3353" t="n">
@@ -44027,7 +44027,7 @@
       </c>
       <c r="B3354" t="inlineStr">
         <is>
-          <t>GEORGE PILKINGTON</t>
+          <t>JORDI XAMMAR, NORA BRUGMAN</t>
         </is>
       </c>
       <c r="C3354" t="n">
@@ -44040,7 +44040,7 @@
       </c>
       <c r="B3355" t="inlineStr">
         <is>
-          <t>CASEY IMENEO</t>
+          <t>WIKTORIA GOLEBIOWSKA</t>
         </is>
       </c>
       <c r="C3355" t="n">
@@ -44053,7 +44053,7 @@
       </c>
       <c r="B3356" t="inlineStr">
         <is>
-          <t>FILIP JURIIC</t>
+          <t>GIORGIA DELLA VALLE</t>
         </is>
       </c>
       <c r="C3356" t="n">
@@ -44066,7 +44066,7 @@
       </c>
       <c r="B3357" t="inlineStr">
         <is>
-          <t>ELISAVET ILIOPOULOU</t>
+          <t>DIMITRI PERONI</t>
         </is>
       </c>
       <c r="C3357" t="n">
@@ -44079,7 +44079,7 @@
       </c>
       <c r="B3358" t="inlineStr">
         <is>
-          <t>YELYZAVETA VYNOHRADOVA</t>
+          <t>CLARA GRAVELY</t>
         </is>
       </c>
       <c r="C3358" t="n">
@@ -44092,7 +44092,7 @@
       </c>
       <c r="B3359" t="inlineStr">
         <is>
-          <t>MAOR BEN HAROSH</t>
+          <t>MIRTHE AKKERMAN</t>
         </is>
       </c>
       <c r="C3359" t="n">
@@ -44105,7 +44105,7 @@
       </c>
       <c r="B3360" t="inlineStr">
         <is>
-          <t>ALENKA VALENCIC</t>
+          <t>MOHIT SAINI</t>
         </is>
       </c>
       <c r="C3360" t="n">
@@ -44118,7 +44118,7 @@
       </c>
       <c r="B3361" t="inlineStr">
         <is>
-          <t>CAROLA  COLASANTO</t>
+          <t>AKSEL HAAVA</t>
         </is>
       </c>
       <c r="C3361" t="n">
@@ -44131,7 +44131,7 @@
       </c>
       <c r="B3362" t="inlineStr">
         <is>
-          <t>MATIAS MONTINHO, MANUELA PAULO</t>
+          <t>MARIA ELENI KALAKONA</t>
         </is>
       </c>
       <c r="C3362" t="n">
@@ -44144,7 +44144,7 @@
       </c>
       <c r="B3363" t="inlineStr">
         <is>
-          <t>MARIA BELEN BAZO</t>
+          <t>STANISLAW  TREPCZYNSKI</t>
         </is>
       </c>
       <c r="C3363" t="n">
@@ -44157,7 +44157,7 @@
       </c>
       <c r="B3364" t="inlineStr">
         <is>
-          <t>FINLEY DICKINSON</t>
+          <t>JEAN BAPTISTE BERNAZ</t>
         </is>
       </c>
       <c r="C3364" t="n">
@@ -44170,7 +44170,7 @@
       </c>
       <c r="B3365" t="inlineStr">
         <is>
-          <t>PEDRO FELIPE ROBLES, CARMINA SOFIA FUENTES</t>
+          <t>MATHEO COGUIEC</t>
         </is>
       </c>
       <c r="C3365" t="n">
@@ -44183,7 +44183,7 @@
       </c>
       <c r="B3366" t="inlineStr">
         <is>
-          <t>SOFIIA NAUMENKO</t>
+          <t>LILLY MAY NIEZABITOWSKA</t>
         </is>
       </c>
       <c r="C3366" t="n">
@@ -44196,7 +44196,7 @@
       </c>
       <c r="B3367" t="inlineStr">
         <is>
-          <t>PETRA MARENDIC</t>
+          <t>REM PULCI MAGEN</t>
         </is>
       </c>
       <c r="C3367" t="n">
@@ -44209,7 +44209,7 @@
       </c>
       <c r="B3368" t="inlineStr">
         <is>
-          <t>JINDONG KONG</t>
+          <t>MATTHEW FLORES</t>
         </is>
       </c>
       <c r="C3368" t="n">
@@ -44222,7 +44222,7 @@
       </c>
       <c r="B3369" t="inlineStr">
         <is>
-          <t>ZOFIA WOJCIK</t>
+          <t>PATRICK CUMMIN</t>
         </is>
       </c>
       <c r="C3369" t="n">
@@ -44235,7 +44235,7 @@
       </c>
       <c r="B3370" t="inlineStr">
         <is>
-          <t>DIEGO BOTIN FLORIAN, TRITTEL PAUL</t>
+          <t>ELENA OETLING RAMIREZ</t>
         </is>
       </c>
       <c r="C3370" t="n">
@@ -44248,7 +44248,7 @@
       </c>
       <c r="B3371" t="inlineStr">
         <is>
-          <t>JANA GERMANI, GIORGIA BERTUZZI</t>
+          <t>PAULA VAN WIERINGEN MASSANET, CLAUDIA SOBRAL LUSQUINOS</t>
         </is>
       </c>
       <c r="C3371" t="n">
@@ -44261,7 +44261,7 @@
       </c>
       <c r="B3372" t="inlineStr">
         <is>
-          <t>YEHOR SAMARIN, YELYZAVETA VASYLENKO</t>
+          <t>GEORGE PILKINGTON</t>
         </is>
       </c>
       <c r="C3372" t="n">
@@ -44274,7 +44274,7 @@
       </c>
       <c r="B3373" t="inlineStr">
         <is>
-          <t>ZACHEE WAYAG</t>
+          <t>KIKO PEIRO</t>
         </is>
       </c>
       <c r="C3373" t="n">
@@ -44287,7 +44287,7 @@
       </c>
       <c r="B3374" t="inlineStr">
         <is>
-          <t>DENISE HELENA RUI PARRUQUE, ALCIDIO PORTUGAL ALMEIDA LINO</t>
+          <t>KENNETH FREDERIKSEN</t>
         </is>
       </c>
       <c r="C3374" t="n">
@@ -44300,7 +44300,7 @@
       </c>
       <c r="B3375" t="inlineStr">
         <is>
-          <t>BELEN TAVELLA, JOAQUIN TARASIDO</t>
+          <t>SEBASTIEN SCHNEITER, ARNO DE PLANTA</t>
         </is>
       </c>
       <c r="C3375" t="n">
@@ -44313,7 +44313,7 @@
       </c>
       <c r="B3376" t="inlineStr">
         <is>
-          <t>DING MINGLIANG, ZHANG WENWEI</t>
+          <t>CAROLA  COLASANTO</t>
         </is>
       </c>
       <c r="C3376" t="n">
@@ -44326,7 +44326,7 @@
       </c>
       <c r="B3377" t="inlineStr">
         <is>
-          <t>WILLEM WIERSEMA</t>
+          <t>THEO REVIL, YANN JAUVIN</t>
         </is>
       </c>
       <c r="C3377" t="n">
@@ -44339,7 +44339,7 @@
       </c>
       <c r="B3378" t="inlineStr">
         <is>
-          <t>LARA MERTEN</t>
+          <t>JAN PERNARCIC, GIOVANNI SANDRINI</t>
         </is>
       </c>
       <c r="C3378" t="n">
@@ -44352,7 +44352,7 @@
       </c>
       <c r="B3379" t="inlineStr">
         <is>
-          <t>ALEJANDRO CLIMENT</t>
+          <t>SHINGEN FURUYA, AKIRA TAKAYANAGI</t>
         </is>
       </c>
       <c r="C3379" t="n">
@@ -44365,7 +44365,7 @@
       </c>
       <c r="B3380" t="inlineStr">
         <is>
-          <t>SAMANTHA EDWARDS</t>
+          <t>DUKO BOS</t>
         </is>
       </c>
       <c r="C3380" t="n">
@@ -44378,7 +44378,7 @@
       </c>
       <c r="B3381" t="inlineStr">
         <is>
-          <t>JOSEFINE NOJGAARD , ESTHER BOJSEN-MOLLER</t>
+          <t>ISHWARIYA GANESH</t>
         </is>
       </c>
       <c r="C3381" t="n">
@@ -44391,7 +44391,7 @@
       </c>
       <c r="B3382" t="inlineStr">
         <is>
-          <t>FILLAH KARIM</t>
+          <t>SHAI KAKON</t>
         </is>
       </c>
       <c r="C3382" t="n">
@@ -44404,7 +44404,7 @@
       </c>
       <c r="B3383" t="inlineStr">
         <is>
-          <t>DANIEL COSTANDI</t>
+          <t>CESARE BARABINO</t>
         </is>
       </c>
       <c r="C3383" t="n">
@@ -44417,7 +44417,7 @@
       </c>
       <c r="B3384" t="inlineStr">
         <is>
-          <t>LOURENCO MATEUS</t>
+          <t>JIANYONG XU, YANI XU</t>
         </is>
       </c>
       <c r="C3384" t="n">
@@ -44430,7 +44430,7 @@
       </c>
       <c r="B3385" t="inlineStr">
         <is>
-          <t>ARIE MOFFAT, HUNTER HOY</t>
+          <t>MARINA ESCUDERO NEGRON</t>
         </is>
       </c>
       <c r="C3385" t="n">
@@ -44443,7 +44443,7 @@
       </c>
       <c r="B3386" t="inlineStr">
         <is>
-          <t>SACHIN GANESH</t>
+          <t>TRISTEN ERIK  KIVI</t>
         </is>
       </c>
       <c r="C3386" t="n">
@@ -44456,7 +44456,7 @@
       </c>
       <c r="B3387" t="inlineStr">
         <is>
-          <t>SANDRA LULIC</t>
+          <t>TEA PETEH</t>
         </is>
       </c>
       <c r="C3387" t="n">
@@ -44469,7 +44469,7 @@
       </c>
       <c r="B3388" t="inlineStr">
         <is>
-          <t>MIHAIL BERBEROV</t>
+          <t>MYKHAILO BILOHORODSKYI, POLINA ZATOCHNA</t>
         </is>
       </c>
       <c r="C3388" t="n">
@@ -44482,7 +44482,7 @@
       </c>
       <c r="B3389" t="inlineStr">
         <is>
-          <t>LOUKIANOS ZAMIT</t>
+          <t>MARIA JOSE PONCEL MAURIN</t>
         </is>
       </c>
       <c r="C3389" t="n">
@@ -44495,7 +44495,7 @@
       </c>
       <c r="B3390" t="inlineStr">
         <is>
-          <t>CAROLINA ALBANO</t>
+          <t>MARIJA ANDELA DE MICHELI-VITTURI, MIHAELA ZJENA DE MICHELI-VITTURI</t>
         </is>
       </c>
       <c r="C3390" t="n">
@@ -44508,7 +44508,7 @@
       </c>
       <c r="B3391" t="inlineStr">
         <is>
-          <t>ERWAN FISCHER, CLEMENT PEQUIN</t>
+          <t>KAARLE TAPPER</t>
         </is>
       </c>
       <c r="C3391" t="n">
@@ -44521,7 +44521,7 @@
       </c>
       <c r="B3392" t="inlineStr">
         <is>
-          <t>MARCELO CAIRO</t>
+          <t>LUKE ELLIOTT</t>
         </is>
       </c>
       <c r="C3392" t="n">
@@ -44534,7 +44534,7 @@
       </c>
       <c r="B3393" t="inlineStr">
         <is>
-          <t>GUILLEM SEGU GIRO</t>
+          <t>KAZUMASA SEGAWA</t>
         </is>
       </c>
       <c r="C3393" t="n">
@@ -44547,7 +44547,7 @@
       </c>
       <c r="B3394" t="inlineStr">
         <is>
-          <t>ENRICO TANFERNA</t>
+          <t>MARINA SERRANO CASTRO</t>
         </is>
       </c>
       <c r="C3394" t="n">
@@ -44560,7 +44560,7 @@
       </c>
       <c r="B3395" t="inlineStr">
         <is>
-          <t>YOGEV ALCALAY</t>
+          <t>ANIL GARNIER</t>
         </is>
       </c>
       <c r="C3395" t="n">
@@ -44573,7 +44573,7 @@
       </c>
       <c r="B3396" t="inlineStr">
         <is>
-          <t>MATTHEW FLORES</t>
+          <t>SANDRO PORTUNE</t>
         </is>
       </c>
       <c r="C3396" t="n">
@@ -44586,7 +44586,7 @@
       </c>
       <c r="B3397" t="inlineStr">
         <is>
-          <t>VALTTERI UUSITALO</t>
+          <t>GIOVANNI DE PAULI</t>
         </is>
       </c>
       <c r="C3397" t="n">
@@ -44599,7 +44599,7 @@
       </c>
       <c r="B3398" t="inlineStr">
         <is>
-          <t>TYTUS BUTOWSKI, BORYS PODUMIS</t>
+          <t>SHEILA MARTINEZ</t>
         </is>
       </c>
       <c r="C3398" t="n">
@@ -44612,7 +44612,7 @@
       </c>
       <c r="B3399" t="inlineStr">
         <is>
-          <t>LUCAS RUAL, EMILE AMOROS</t>
+          <t>HELENA WOLFF</t>
         </is>
       </c>
       <c r="C3399" t="n">
@@ -44625,7 +44625,7 @@
       </c>
       <c r="B3400" t="inlineStr">
         <is>
-          <t>VINCENT PETER</t>
+          <t>DYLAN FORSYTH</t>
         </is>
       </c>
       <c r="C3400" t="n">
@@ -44638,7 +44638,7 @@
       </c>
       <c r="B3401" t="inlineStr">
         <is>
-          <t>PEDRO FERNANDEZ</t>
+          <t>PARIS HENKEN, ANNA TOBIAS</t>
         </is>
       </c>
       <c r="C3401" t="n">
@@ -44651,7 +44651,7 @@
       </c>
       <c r="B3402" t="inlineStr">
         <is>
-          <t>KATRINA MICALLEF</t>
+          <t>MATIAS MONTINHO, MANUELA PAULO</t>
         </is>
       </c>
       <c r="C3402" t="n">
@@ -44664,7 +44664,7 @@
       </c>
       <c r="B3403" t="inlineStr">
         <is>
-          <t>DIOGO COSTA, CAROLINA JOAO</t>
+          <t>LUCAS RUAL, EMILE AMOROS</t>
         </is>
       </c>
       <c r="C3403" t="n">
@@ -44677,7 +44677,7 @@
       </c>
       <c r="B3404" t="inlineStr">
         <is>
-          <t>CORENTIN GOULON, TIMOTHEE DEPERY</t>
+          <t>CARLOS ESPI</t>
         </is>
       </c>
       <c r="C3404" t="n">
@@ -44690,7 +44690,7 @@
       </c>
       <c r="B3405" t="inlineStr">
         <is>
-          <t>YIGIT YALCIN CITAK</t>
+          <t>OKYANUS ARIKAN</t>
         </is>
       </c>
       <c r="C3405" t="n">
@@ -44703,7 +44703,7 @@
       </c>
       <c r="B3406" t="inlineStr">
         <is>
-          <t>YUTA IRIE</t>
+          <t>THOMAS FARLEY</t>
         </is>
       </c>
       <c r="C3406" t="n">
@@ -44716,7 +44716,7 @@
       </c>
       <c r="B3407" t="inlineStr">
         <is>
-          <t>WUNIU AYU</t>
+          <t>ELLIOTT WELLS BILLY, VENNIS-OZANNE</t>
         </is>
       </c>
       <c r="C3407" t="n">
@@ -44729,7 +44729,7 @@
       </c>
       <c r="B3408" t="inlineStr">
         <is>
-          <t>DAISY COLLINGRIDGE</t>
+          <t>PEDRO FERNANDEZ</t>
         </is>
       </c>
       <c r="C3408" t="n">
@@ -44742,7 +44742,7 @@
       </c>
       <c r="B3409" t="inlineStr">
         <is>
-          <t>JIANYONG XU, YANI XU</t>
+          <t>SAKI MATSUNAE, ERI HATAYAMA</t>
         </is>
       </c>
       <c r="C3409" t="n">
@@ -44755,7 +44755,7 @@
       </c>
       <c r="B3410" t="inlineStr">
         <is>
-          <t>TIM</t>
+          <t>EMILE  ROULLET</t>
         </is>
       </c>
       <c r="C3410" t="n">
@@ -44768,7 +44768,7 @@
       </c>
       <c r="B3411" t="inlineStr">
         <is>
-          <t>MARIA VLACHOU</t>
+          <t>PANAGIOTIS SPANOS</t>
         </is>
       </c>
       <c r="C3411" t="n">
@@ -44781,7 +44781,7 @@
       </c>
       <c r="B3412" t="inlineStr">
         <is>
-          <t>BRUNA MARTINELLI CESARIO DE MELLO</t>
+          <t>LARA MERTEN</t>
         </is>
       </c>
       <c r="C3412" t="n">
@@ -44794,7 +44794,7 @@
       </c>
       <c r="B3413" t="inlineStr">
         <is>
-          <t>JOAQUIN BLANCO ALBALAT</t>
+          <t>DIMITRIOS ANASTASIADIS</t>
         </is>
       </c>
       <c r="C3413" t="n">
@@ -44807,7 +44807,7 @@
       </c>
       <c r="B3414" t="inlineStr">
         <is>
-          <t>PETRA MASTELIC</t>
+          <t>EMIL BENGTSON</t>
         </is>
       </c>
       <c r="C3414" t="n">
@@ -44820,7 +44820,7 @@
       </c>
       <c r="B3415" t="inlineStr">
         <is>
-          <t>HERNAN UMPIERRE, FERNANDO DIZ</t>
+          <t>MARLA BERGMANN, HANNA WILLE</t>
         </is>
       </c>
       <c r="C3415" t="n">
@@ -44833,7 +44833,7 @@
       </c>
       <c r="B3416" t="inlineStr">
         <is>
-          <t>STEVE GUNTHER</t>
+          <t>MALO KENNISH, ANATOLE MARTIN</t>
         </is>
       </c>
       <c r="C3416" t="n">
@@ -44846,7 +44846,7 @@
       </c>
       <c r="B3417" t="inlineStr">
         <is>
-          <t>HAMISH CRABB</t>
+          <t>BERKAY ABAY</t>
         </is>
       </c>
       <c r="C3417" t="n">
@@ -44859,7 +44859,7 @@
       </c>
       <c r="B3418" t="inlineStr">
         <is>
-          <t>KAI WOLGRAM</t>
+          <t>ANNA VASILIEVA</t>
         </is>
       </c>
       <c r="C3418" t="n">
@@ -44872,7 +44872,7 @@
       </c>
       <c r="B3419" t="inlineStr">
         <is>
-          <t>MARINA ESCUDERO NEGRON</t>
+          <t>CHRISTINA MARIA MENI</t>
         </is>
       </c>
       <c r="C3419" t="n">
@@ -44885,7 +44885,7 @@
       </c>
       <c r="B3420" t="inlineStr">
         <is>
-          <t>LUC CHEVRIER</t>
+          <t>JAMES PERCIVAL COOKE</t>
         </is>
       </c>
       <c r="C3420" t="n">
@@ -44898,7 +44898,7 @@
       </c>
       <c r="B3421" t="inlineStr">
         <is>
-          <t>LOUIS GARINO</t>
+          <t>LINDA DOKOUPILOVA</t>
         </is>
       </c>
       <c r="C3421" t="n">
@@ -44911,7 +44911,7 @@
       </c>
       <c r="B3422" t="inlineStr">
         <is>
-          <t>ILIJA MARKOVIC</t>
+          <t>GAYA DATIASHVILI</t>
         </is>
       </c>
       <c r="C3422" t="n">
@@ -44924,7 +44924,7 @@
       </c>
       <c r="B3423" t="inlineStr">
         <is>
-          <t>EDWARD REID</t>
+          <t>ANDREAS KRABBE CHRISTENSEN</t>
         </is>
       </c>
       <c r="C3423" t="n">
@@ -44937,7 +44937,7 @@
       </c>
       <c r="B3424" t="inlineStr">
         <is>
-          <t>WIKTORIA GOLEBIOWSKA</t>
+          <t>DIOGO COSTA, CAROLINA JOAO</t>
         </is>
       </c>
       <c r="C3424" t="n">
@@ -44950,7 +44950,7 @@
       </c>
       <c r="B3425" t="inlineStr">
         <is>
-          <t>MEGUMI ISEDA</t>
+          <t>QIBIN HUANG</t>
         </is>
       </c>
       <c r="C3425" t="n">
@@ -44963,7 +44963,7 @@
       </c>
       <c r="B3426" t="inlineStr">
         <is>
-          <t>TOMASZ BENDLEWSKI</t>
+          <t>MAX STINGELE, LINOV SCHEEL</t>
         </is>
       </c>
       <c r="C3426" t="n">
@@ -44976,7 +44976,7 @@
       </c>
       <c r="B3427" t="inlineStr">
         <is>
-          <t>ANDRE REGUERO, ANDRE GUARAGNA</t>
+          <t>TAEHOON LEE</t>
         </is>
       </c>
       <c r="C3427" t="n">
@@ -44989,7 +44989,7 @@
       </c>
       <c r="B3428" t="inlineStr">
         <is>
-          <t>LUCIANA CARDOZO</t>
+          <t>YVES MERMOD, MAJA SIEGENTHALER</t>
         </is>
       </c>
       <c r="C3428" t="n">
@@ -45002,7 +45002,7 @@
       </c>
       <c r="B3429" t="inlineStr">
         <is>
-          <t>KJELL HASCHEN, IVEN FROMM</t>
+          <t>BEATA DOKOUPILOVA</t>
         </is>
       </c>
       <c r="C3429" t="n">
@@ -45015,7 +45015,7 @@
       </c>
       <c r="B3430" t="inlineStr">
         <is>
-          <t>BERNAT TOMAS</t>
+          <t>SPYROS PROVELEGIOS</t>
         </is>
       </c>
       <c r="C3430" t="n">
@@ -45028,7 +45028,7 @@
       </c>
       <c r="B3431" t="inlineStr">
         <is>
-          <t>GASPAR PETIT</t>
+          <t>MIRANDA PAPADAKI</t>
         </is>
       </c>
       <c r="C3431" t="n">
@@ -45041,7 +45041,7 @@
       </c>
       <c r="B3432" t="inlineStr">
         <is>
-          <t>LENNART KUSS</t>
+          <t>NOCETI KLEPACKA ZOFIA</t>
         </is>
       </c>
       <c r="C3432" t="n">
@@ -45054,7 +45054,7 @@
       </c>
       <c r="B3433" t="inlineStr">
         <is>
-          <t>JAKOB MEGGENDORFER, ANDREAS SPRANGER</t>
+          <t>YOSHIHIRO SUZUKI</t>
         </is>
       </c>
       <c r="C3433" t="n">
@@ -45067,7 +45067,7 @@
       </c>
       <c r="B3434" t="inlineStr">
         <is>
-          <t>LINDA DOKOUPILOVA</t>
+          <t>LUCY DAVIS</t>
         </is>
       </c>
       <c r="C3434" t="n">
@@ -45080,7 +45080,7 @@
       </c>
       <c r="B3435" t="inlineStr">
         <is>
-          <t>DENIZ CINAR, LARA NALBANTOGLU</t>
+          <t>ASCENSION ROCA DE TOGORES BENABENT</t>
         </is>
       </c>
       <c r="C3435" t="n">
@@ -45093,7 +45093,7 @@
       </c>
       <c r="B3436" t="inlineStr">
         <is>
-          <t>PEP CAZADOR</t>
+          <t>ALICIA FRAS ELENA, BARRIO GARCIA</t>
         </is>
       </c>
       <c r="C3436" t="n">
@@ -45106,7 +45106,7 @@
       </c>
       <c r="B3437" t="inlineStr">
         <is>
-          <t>REM PULCI MAGEN</t>
+          <t>NEUS BALLESTER, CARLOTA GARCIA</t>
         </is>
       </c>
       <c r="C3437" t="n">
@@ -45119,7 +45119,7 @@
       </c>
       <c r="B3438" t="inlineStr">
         <is>
-          <t>PAWEL TARNOWSKI</t>
+          <t>TIMO COUPEK</t>
         </is>
       </c>
       <c r="C3438" t="n">
@@ -45132,7 +45132,7 @@
       </c>
       <c r="B3439" t="inlineStr">
         <is>
-          <t>ALICIA FRAS ELENA, BARRIO GARCIA</t>
+          <t>NICOLE VAN DER VELDEN VIZCAYA</t>
         </is>
       </c>
       <c r="C3439" t="n">
@@ -45145,7 +45145,7 @@
       </c>
       <c r="B3440" t="inlineStr">
         <is>
-          <t>PIA CONRADI</t>
+          <t>BARBARA WINAU ORDINAS</t>
         </is>
       </c>
       <c r="C3440" t="n">
@@ -45158,7 +45158,7 @@
       </c>
       <c r="B3441" t="inlineStr">
         <is>
-          <t>TEA PETEH</t>
+          <t>VALTTERI UUSITALO</t>
         </is>
       </c>
       <c r="C3441" t="n">
@@ -45171,7 +45171,7 @@
       </c>
       <c r="B3442" t="inlineStr">
         <is>
-          <t>PATRICK CUMMIN</t>
+          <t>ATTILIO BORIO</t>
         </is>
       </c>
       <c r="C3442" t="n">
@@ -45184,7 +45184,7 @@
       </c>
       <c r="B3443" t="inlineStr">
         <is>
-          <t>SAMUEL ABEN</t>
+          <t>HAMISH CRABB</t>
         </is>
       </c>
       <c r="C3443" t="n">
@@ -45197,7 +45197,7 @@
       </c>
       <c r="B3444" t="inlineStr">
         <is>
-          <t>BAUDOUIN MOTTE</t>
+          <t>HONOKA MIURA</t>
         </is>
       </c>
       <c r="C3444" t="n">
@@ -45210,7 +45210,7 @@
       </c>
       <c r="B3445" t="inlineStr">
         <is>
-          <t>ANATOL SASSI</t>
+          <t>KLEOPATRA ANASTASSIOU</t>
         </is>
       </c>
       <c r="C3445" t="n">
@@ -45223,7 +45223,7 @@
       </c>
       <c r="B3446" t="inlineStr">
         <is>
-          <t>JEAN BAPTISTE BERNAZ</t>
+          <t>JOSEPHINE HEEGAARD</t>
         </is>
       </c>
       <c r="C3446" t="n">
@@ -45236,7 +45236,7 @@
       </c>
       <c r="B3447" t="inlineStr">
         <is>
-          <t>NETHRA KUMANAN</t>
+          <t>PATROKLOS THEODOROS TSARAMYRSIS</t>
         </is>
       </c>
       <c r="C3447" t="n">
@@ -45249,7 +45249,7 @@
       </c>
       <c r="B3448" t="inlineStr">
         <is>
-          <t>ILIJA MARKOVIAE</t>
+          <t>VITA HEATHCOTE, CHRIS GRUBE</t>
         </is>
       </c>
       <c r="C3448" t="n">
@@ -45262,7 +45262,7 @@
       </c>
       <c r="B3449" t="inlineStr">
         <is>
-          <t>TEETOS TAKSINAPAN</t>
+          <t>BELEN TAVELLA, JOAQUIN TARASIDO</t>
         </is>
       </c>
       <c r="C3449" t="n">
@@ -45275,7 +45275,7 @@
       </c>
       <c r="B3450" t="inlineStr">
         <is>
-          <t>SEBASTIAN DUCOS</t>
+          <t>LOURENCO MATEUS</t>
         </is>
       </c>
       <c r="C3450" t="n">
@@ -45288,7 +45288,7 @@
       </c>
       <c r="B3451" t="inlineStr">
         <is>
-          <t>GIACOMO FERRARI, ALESSANDRA DUBBINI</t>
+          <t>ZAN LUKA ZELKO</t>
         </is>
       </c>
       <c r="C3451" t="n">
@@ -45301,7 +45301,7 @@
       </c>
       <c r="B3452" t="inlineStr">
         <is>
-          <t>ANDY  BROWN</t>
+          <t>PETRA MARENDIC</t>
         </is>
       </c>
       <c r="C3452" t="n">
@@ -45314,7 +45314,7 @@
       </c>
       <c r="B3453" t="inlineStr">
         <is>
-          <t>MARIA ELENI KALAKONA</t>
+          <t>NIKOLA  GIRKE</t>
         </is>
       </c>
       <c r="C3453" t="n">
@@ -45327,7 +45327,7 @@
       </c>
       <c r="B3454" t="inlineStr">
         <is>
-          <t>GUSTAV AASHOLM-BRADLEY, FREDERIK RAGAN MELBYE</t>
+          <t>ANDRE REGUERO, ANDRE GUARAGNA</t>
         </is>
       </c>
       <c r="C3454" t="n">
@@ -45340,7 +45340,7 @@
       </c>
       <c r="B3455" t="inlineStr">
         <is>
-          <t>CLARA GRAVELY</t>
+          <t>HENRIQUE HADDAD, ISABEL SWAN</t>
         </is>
       </c>
       <c r="C3455" t="n">
@@ -45353,7 +45353,7 @@
       </c>
       <c r="B3456" t="inlineStr">
         <is>
-          <t>LINE FLEM HOEST</t>
+          <t>LUCY BILGER</t>
         </is>
       </c>
       <c r="C3456" t="n">
@@ -45366,7 +45366,7 @@
       </c>
       <c r="B3457" t="inlineStr">
         <is>
-          <t>GUSTAVO ABDULKLECH, NICOLAS BERNAL</t>
+          <t>MARIE EVE MAYRAND</t>
         </is>
       </c>
       <c r="C3457" t="n">
@@ -45379,7 +45379,7 @@
       </c>
       <c r="B3458" t="inlineStr">
         <is>
-          <t>SAMUEL OLIVER SILLS</t>
+          <t>SAKAI AKIRA, AYLSWORTH RUSSELL</t>
         </is>
       </c>
       <c r="C3458" t="n">
@@ -45392,7 +45392,7 @@
       </c>
       <c r="B3459" t="inlineStr">
         <is>
-          <t>KRISTINA BOJA</t>
+          <t>JOAQUIN BLANCO ALBALAT</t>
         </is>
       </c>
       <c r="C3459" t="n">
@@ -45405,7 +45405,7 @@
       </c>
       <c r="B3460" t="inlineStr">
         <is>
-          <t>IGOR LEWINSKI</t>
+          <t>GUILLEM SEGU GIRO</t>
         </is>
       </c>
       <c r="C3460" t="n">
@@ -45418,7 +45418,7 @@
       </c>
       <c r="B3461" t="inlineStr">
         <is>
-          <t>TATIANI BOUGIATIOTI</t>
+          <t>SAMUEL BENEYTO</t>
         </is>
       </c>
       <c r="C3461" t="n">
@@ -45431,7 +45431,7 @@
       </c>
       <c r="B3462" t="inlineStr">
         <is>
-          <t>NIA JERWOOD, CONOR NICHOLAS</t>
+          <t>JUAN MAEGLI</t>
         </is>
       </c>
       <c r="C3462" t="n">
@@ -45444,7 +45444,7 @@
       </c>
       <c r="B3463" t="inlineStr">
         <is>
-          <t>FORD MCCANN</t>
+          <t>ELEANOR ALDRIDGE</t>
         </is>
       </c>
       <c r="C3463" t="n">
@@ -45457,7 +45457,7 @@
       </c>
       <c r="B3464" t="inlineStr">
         <is>
-          <t>JOHN GORDON</t>
+          <t>SOPHIE RENNIE</t>
         </is>
       </c>
       <c r="C3464" t="n">
@@ -45470,7 +45470,7 @@
       </c>
       <c r="B3465" t="inlineStr">
         <is>
-          <t>POULIQUEN YUN</t>
+          <t>MARIA BELEN BAZO</t>
         </is>
       </c>
       <c r="C3465" t="n">
@@ -45483,7 +45483,7 @@
       </c>
       <c r="B3466" t="inlineStr">
         <is>
-          <t>SOPHIE RENNIE</t>
+          <t>DENIZ CINAR, LARA NALBANTOGLU</t>
         </is>
       </c>
       <c r="C3466" t="n">
@@ -45496,7 +45496,7 @@
       </c>
       <c r="B3467" t="inlineStr">
         <is>
-          <t>GUILHERME  PLENTZ</t>
+          <t>YULONG QIU</t>
         </is>
       </c>
       <c r="C3467" t="n">
@@ -45509,7 +45509,7 @@
       </c>
       <c r="B3468" t="inlineStr">
         <is>
-          <t>CANNELLE OPSTAELE</t>
+          <t>JOSEFIN OLSSON</t>
         </is>
       </c>
       <c r="C3468" t="n">
@@ -45522,7 +45522,7 @@
       </c>
       <c r="B3469" t="inlineStr">
         <is>
-          <t>MICHAEL LEIGH</t>
+          <t>BRUNO GASPIC</t>
         </is>
       </c>
       <c r="C3469" t="n">
@@ -45535,7 +45535,7 @@
       </c>
       <c r="B3470" t="inlineStr">
         <is>
-          <t>CARLOTTA RIZZARDI</t>
+          <t>BRUNA MARTINELLI CESARIO DE MELLO</t>
         </is>
       </c>
       <c r="C3470" t="n">
@@ -45548,7 +45548,7 @@
       </c>
       <c r="B3471" t="inlineStr">
         <is>
-          <t>CESARE BARABINO</t>
+          <t>AI YOSHIDA, YUGO YOSHIDA</t>
         </is>
       </c>
       <c r="C3471" t="n">
@@ -45561,7 +45561,7 @@
       </c>
       <c r="B3472" t="inlineStr">
         <is>
-          <t>GAYA DATIASHVILI</t>
+          <t>MILLIE IRISH, SZYMON MATYJASZCZUK</t>
         </is>
       </c>
       <c r="C3472" t="n">
@@ -45574,7 +45574,7 @@
       </c>
       <c r="B3473" t="inlineStr">
         <is>
-          <t>MICHAEL PALIOS</t>
+          <t>ROSA DONNER, NIKLAS HABERL</t>
         </is>
       </c>
       <c r="C3473" t="n">
@@ -45587,7 +45587,7 @@
       </c>
       <c r="B3474" t="inlineStr">
         <is>
-          <t>JULIAN TAYLOR</t>
+          <t>JINDONG KONG</t>
         </is>
       </c>
       <c r="C3474" t="n">
@@ -45600,7 +45600,7 @@
       </c>
       <c r="B3475" t="inlineStr">
         <is>
-          <t>LILLY MAY NIEZABITOWSKA</t>
+          <t>IGOR LEWINSKI</t>
         </is>
       </c>
       <c r="C3475" t="n">
@@ -45613,7 +45613,7 @@
       </c>
       <c r="B3476" t="inlineStr">
         <is>
-          <t>CHRIS THORPE</t>
+          <t>GASPAR PETIT</t>
         </is>
       </c>
       <c r="C3476" t="n">
@@ -45626,7 +45626,7 @@
       </c>
       <c r="B3477" t="inlineStr">
         <is>
-          <t>AGNIESZKA PAWLOWSKA, BARTEK SZLIJA</t>
+          <t>ADA TAN</t>
         </is>
       </c>
       <c r="C3477" t="n">
@@ -45639,7 +45639,7 @@
       </c>
       <c r="B3478" t="inlineStr">
         <is>
-          <t>LEONARD COLLADO</t>
+          <t>YANNICK LEFEBVRE, YOUENN BERTIN</t>
         </is>
       </c>
       <c r="C3478" t="n">
@@ -45652,7 +45652,7 @@
       </c>
       <c r="B3479" t="inlineStr">
         <is>
-          <t>GIOVANNI DE PAULI</t>
+          <t>GABRIELLA KIDD</t>
         </is>
       </c>
       <c r="C3479" t="n">
@@ -45665,7 +45665,7 @@
       </c>
       <c r="B3480" t="inlineStr">
         <is>
-          <t>STEFAN ELLIOTT SHIRCORE</t>
+          <t>MELINA PAPPA, NIKOLAS GIOTOPOULOS</t>
         </is>
       </c>
       <c r="C3480" t="n">
@@ -45678,7 +45678,7 @@
       </c>
       <c r="B3481" t="inlineStr">
         <is>
-          <t>YOSHIHIRO SUZUKI</t>
+          <t>DING MINGLIANG, ZHANG WENWEI</t>
         </is>
       </c>
       <c r="C3481" t="n">
@@ -45691,7 +45691,7 @@
       </c>
       <c r="B3482" t="inlineStr">
         <is>
-          <t>NOEL LAUKKANEN</t>
+          <t>KACPER PASZEK, IGA WIELCZYK</t>
         </is>
       </c>
       <c r="C3482" t="n">
@@ -45704,7 +45704,7 @@
       </c>
       <c r="B3483" t="inlineStr">
         <is>
-          <t>SANDRO PORTUNE</t>
+          <t>ALEKSANDRA WASIEWICZ</t>
         </is>
       </c>
       <c r="C3483" t="n">
@@ -45717,7 +45717,7 @@
       </c>
       <c r="B3484" t="inlineStr">
         <is>
-          <t>EMIL BENGTSON</t>
+          <t>NIA JERWOOD, CONOR NICHOLAS</t>
         </is>
       </c>
       <c r="C3484" t="n">
@@ -45730,7 +45730,7 @@
       </c>
       <c r="B3485" t="inlineStr">
         <is>
-          <t>VITA HEATHCOTE, CHRIS GRUBE</t>
+          <t>STEVE GUNTHER</t>
         </is>
       </c>
       <c r="C3485" t="n">
@@ -45743,7 +45743,7 @@
       </c>
       <c r="B3486" t="inlineStr">
         <is>
-          <t>SAM KING</t>
+          <t>BAUDOUIN MOTTE</t>
         </is>
       </c>
       <c r="C3486" t="n">
@@ -45756,7 +45756,7 @@
       </c>
       <c r="B3487" t="inlineStr">
         <is>
-          <t>MALO KENNISH, ANATOLE MARTIN</t>
+          <t>JOSEPHINE P W FREDERIKSEN, LAURA STEENSTRUP ZEEBERG</t>
         </is>
       </c>
       <c r="C3487" t="n">
@@ -45769,7 +45769,7 @@
       </c>
       <c r="B3488" t="inlineStr">
         <is>
-          <t>LUCA VALENTINO</t>
+          <t>TEETOS TAKSINAPAN</t>
         </is>
       </c>
       <c r="C3488" t="n">
@@ -45782,7 +45782,7 @@
       </c>
       <c r="B3489" t="inlineStr">
         <is>
-          <t>SAMUEL BENEYTO</t>
+          <t>AGNIESZKA PAWLOWSKA, BARTEK SZLIJA</t>
         </is>
       </c>
       <c r="C3489" t="n">
@@ -45795,7 +45795,7 @@
       </c>
       <c r="B3490" t="inlineStr">
         <is>
-          <t>BEN FLOWER</t>
+          <t>FUJIKO ONISHI</t>
         </is>
       </c>
       <c r="C3490" t="n">
@@ -45808,7 +45808,7 @@
       </c>
       <c r="B3491" t="inlineStr">
         <is>
-          <t>ELENA OETLING RAMIREZ</t>
+          <t>PAOLO FREDDI</t>
         </is>
       </c>
       <c r="C3491" t="n">
@@ -45821,7 +45821,7 @@
       </c>
       <c r="B3492" t="inlineStr">
         <is>
-          <t>VYRON KOKKALANIS</t>
+          <t>SEBASTIAN DUCOS</t>
         </is>
       </c>
       <c r="C3492" t="n">
@@ -45834,7 +45834,7 @@
       </c>
       <c r="B3493" t="inlineStr">
         <is>
-          <t>ANTUN TOMASEVIC</t>
+          <t>VALADE LOMANE, JULIEN BUNEL</t>
         </is>
       </c>
       <c r="C3493" t="n">
@@ -45847,7 +45847,7 @@
       </c>
       <c r="B3494" t="inlineStr">
         <is>
-          <t>ROBBY MEEK</t>
+          <t>NIKOLE BARNES, TED MCDONOUGH</t>
         </is>
       </c>
       <c r="C3494" t="n">
@@ -45860,7 +45860,7 @@
       </c>
       <c r="B3495" t="inlineStr">
         <is>
-          <t>JASON KEFALLONITIS</t>
+          <t>JOSEFINE NOJGAARD , ESTHER BOJSEN-MOLLER</t>
         </is>
       </c>
       <c r="C3495" t="n">
@@ -45873,7 +45873,7 @@
       </c>
       <c r="B3496" t="inlineStr">
         <is>
-          <t>MARINA SERRANO CASTRO</t>
+          <t>JASON KEFALLONITIS</t>
         </is>
       </c>
       <c r="C3496" t="n">
@@ -45886,7 +45886,7 @@
       </c>
       <c r="B3497" t="inlineStr">
         <is>
-          <t>MAOR BENHAROCH</t>
+          <t>ZOFIA WOJCIK</t>
         </is>
       </c>
       <c r="C3497" t="n">
@@ -45899,7 +45899,7 @@
       </c>
       <c r="B3498" t="inlineStr">
         <is>
-          <t>KLEOPATRA ANASTASSIOU</t>
+          <t>ERIK NORLEN</t>
         </is>
       </c>
       <c r="C3498" t="n">
@@ -45912,7 +45912,7 @@
       </c>
       <c r="B3499" t="inlineStr">
         <is>
-          <t>ENDRE FUNNEMARK FUNNEMARK</t>
+          <t>MARIT BOUWMEESTER</t>
         </is>
       </c>
       <c r="C3499" t="n">
@@ -45925,7 +45925,7 @@
       </c>
       <c r="B3500" t="inlineStr">
         <is>
-          <t>MARIA SOL BRANZ CRESPO, JULIA PANTIN</t>
+          <t>LOUIS GARINO</t>
         </is>
       </c>
       <c r="C3500" t="n">
@@ -45938,7 +45938,7 @@
       </c>
       <c r="B3501" t="inlineStr">
         <is>
-          <t>THOMAS FARLEY</t>
+          <t>ANASTASIA KASKANTAMI</t>
         </is>
       </c>
       <c r="C3501" t="n">
@@ -45951,7 +45951,7 @@
       </c>
       <c r="B3502" t="inlineStr">
         <is>
-          <t>MATHEO COGUIEC</t>
+          <t>CAROLINA ALBANO</t>
         </is>
       </c>
       <c r="C3502" t="n">
@@ -45964,7 +45964,7 @@
       </c>
       <c r="B3503" t="inlineStr">
         <is>
-          <t>ALEXANDROS IOANNIDIS</t>
+          <t>LAMPROS NIKOLAOS GARMPIS</t>
         </is>
       </c>
       <c r="C3503" t="n">
@@ -45977,7 +45977,7 @@
       </c>
       <c r="B3504" t="inlineStr">
         <is>
-          <t>ALEKSANDRA WASIEWICZ</t>
+          <t>MATEUSZ GWOZDZ, LUKASZ MACHOWSKI</t>
         </is>
       </c>
       <c r="C3504" t="n">
@@ -45990,7 +45990,7 @@
       </c>
       <c r="B3505" t="inlineStr">
         <is>
-          <t>ANASTASIA KASKANTAMI</t>
+          <t>ALISE SANTORUM</t>
         </is>
       </c>
       <c r="C3505" t="n">
@@ -46003,7 +46003,7 @@
       </c>
       <c r="B3506" t="inlineStr">
         <is>
-          <t>SARA SZENTIVANYI</t>
+          <t>NITIPHAT    CHAIWUTTIWET</t>
         </is>
       </c>
       <c r="C3506" t="n">
@@ -46016,7 +46016,7 @@
       </c>
       <c r="B3507" t="inlineStr">
         <is>
-          <t>KAREL RATNIK</t>
+          <t>SOPHIA  MEYER</t>
         </is>
       </c>
       <c r="C3507" t="n">
@@ -46029,7 +46029,7 @@
       </c>
       <c r="B3508" t="inlineStr">
         <is>
-          <t>BERKAY ABAY</t>
+          <t>ANGELO SOLI</t>
         </is>
       </c>
       <c r="C3508" t="n">
@@ -46042,7 +46042,7 @@
       </c>
       <c r="B3509" t="inlineStr">
         <is>
-          <t>SPYROS PROVELEGIOS</t>
+          <t>CHARLOTTE VIDELO</t>
         </is>
       </c>
       <c r="C3509" t="n">
@@ -46055,7 +46055,7 @@
       </c>
       <c r="B3510" t="inlineStr">
         <is>
-          <t>MALTHE EBDRUP, CLEMENT AASHOLM-BRADLEY</t>
+          <t>MARIA VLACHOU</t>
         </is>
       </c>
       <c r="C3510" t="n">
@@ -46068,7 +46068,7 @@
       </c>
       <c r="B3511" t="inlineStr">
         <is>
-          <t>ANA MONCADA</t>
+          <t>IRIS SINGLETON</t>
         </is>
       </c>
       <c r="C3511" t="n">
@@ -46081,7 +46081,7 @@
       </c>
       <c r="B3512" t="inlineStr">
         <is>
-          <t>LUCY DAVIS</t>
+          <t>ELKAN RESHAWN OH</t>
         </is>
       </c>
       <c r="C3512" t="n">
@@ -46094,7 +46094,7 @@
       </c>
       <c r="B3513" t="inlineStr">
         <is>
-          <t>ELYSE AINSWORTH</t>
+          <t>KAI WOLGRAM</t>
         </is>
       </c>
       <c r="C3513" t="n">
@@ -46107,7 +46107,7 @@
       </c>
       <c r="B3514" t="inlineStr">
         <is>
-          <t>ELISA HARTENBERGER</t>
+          <t>GIAN STRAGIOTTI</t>
         </is>
       </c>
       <c r="C3514" t="n">
@@ -46120,7 +46120,7 @@
       </c>
       <c r="B3515" t="inlineStr">
         <is>
-          <t>ELI LIEFTING</t>
+          <t>ENDRE FUNNEMARK FUNNEMARK</t>
         </is>
       </c>
       <c r="C3515" t="n">
@@ -46133,7 +46133,7 @@
       </c>
       <c r="B3516" t="inlineStr">
         <is>
-          <t>LUKAS WALTON KEIM</t>
+          <t>HERMANN TOMASGAARD</t>
         </is>
       </c>
       <c r="C3516" t="n">
@@ -46146,7 +46146,7 @@
       </c>
       <c r="B3517" t="inlineStr">
         <is>
-          <t>MAX STINGELE, LINOV SCHEEL</t>
+          <t>NOEL LAUKKANEN</t>
         </is>
       </c>
       <c r="C3517" t="n">
@@ -46159,7 +46159,7 @@
       </c>
       <c r="B3518" t="inlineStr">
         <is>
-          <t>IRIS SINGLETON</t>
+          <t>FILIP OLSZEWSKI</t>
         </is>
       </c>
       <c r="C3518" t="n">
@@ -46172,7 +46172,7 @@
       </c>
       <c r="B3519" t="inlineStr">
         <is>
-          <t>TOM HOLMES</t>
+          <t>LUKAS WALTON KEIM</t>
         </is>
       </c>
       <c r="C3519" t="n">
@@ -46185,7 +46185,7 @@
       </c>
       <c r="B3520" t="inlineStr">
         <is>
-          <t>ELEANOR ALDRIDGE</t>
+          <t>NIKOLA BANJAC</t>
         </is>
       </c>
       <c r="C3520" t="n">
@@ -46198,7 +46198,7 @@
       </c>
       <c r="B3521" t="inlineStr">
         <is>
-          <t>PATROKLOS THEODOROS TSARAMYRSIS</t>
+          <t>YEHOR SAMARIN, YELYZAVETA VASYLENKO</t>
         </is>
       </c>
       <c r="C3521" t="n">
@@ -46211,7 +46211,7 @@
       </c>
       <c r="B3522" t="inlineStr">
         <is>
-          <t>ERIK NORLEN</t>
+          <t>ISAAC SCHOTTE</t>
         </is>
       </c>
       <c r="C3522" t="n">
@@ -46224,7 +46224,7 @@
       </c>
       <c r="B3523" t="inlineStr">
         <is>
-          <t>ANNA VASILIEVA</t>
+          <t>YU CHEN</t>
         </is>
       </c>
       <c r="C3523" t="n">
@@ -46237,7 +46237,7 @@
       </c>
       <c r="B3524" t="inlineStr">
         <is>
-          <t>JAMES PERCIVAL COOKE</t>
+          <t>DAVID SURKOV</t>
         </is>
       </c>
       <c r="C3524" t="n">
@@ -46250,7 +46250,7 @@
       </c>
       <c r="B3525" t="inlineStr">
         <is>
-          <t>AKSEL HAAVA</t>
+          <t>DAISY COLLINGRIDGE</t>
         </is>
       </c>
       <c r="C3525" t="n">
@@ -46263,7 +46263,7 @@
       </c>
       <c r="B3526" t="inlineStr">
         <is>
-          <t>PIERRE  LE COQ</t>
+          <t>NICOL SEGNINI</t>
         </is>
       </c>
       <c r="C3526" t="n">
@@ -46276,7 +46276,7 @@
       </c>
       <c r="B3527" t="inlineStr">
         <is>
-          <t>JARROD JONES</t>
+          <t>LIAM BRUCE</t>
         </is>
       </c>
       <c r="C3527" t="n">
@@ -46289,7 +46289,7 @@
       </c>
       <c r="B3528" t="inlineStr">
         <is>
-          <t>ANDREAS KRABBE</t>
+          <t>ANDY  BROWN</t>
         </is>
       </c>
       <c r="C3528" t="n">
@@ -46302,7 +46302,7 @@
       </c>
       <c r="B3529" t="inlineStr">
         <is>
-          <t>NICO NAUJOCK</t>
+          <t>BENJAMIN AGANOVIE</t>
         </is>
       </c>
       <c r="C3529" t="n">
@@ -46315,7 +46315,7 @@
       </c>
       <c r="B3530" t="inlineStr">
         <is>
-          <t>MARIE EVE MAYRAND</t>
+          <t>ANDREAS KRABBE</t>
         </is>
       </c>
       <c r="C3530" t="n">
@@ -46328,7 +46328,7 @@
       </c>
       <c r="B3531" t="inlineStr">
         <is>
-          <t>MATILDA TALLURI</t>
+          <t>GEORGIA KATSOULI</t>
         </is>
       </c>
       <c r="C3531" t="n">
@@ -46341,7 +46341,7 @@
       </c>
       <c r="B3532" t="inlineStr">
         <is>
-          <t>GEORGIA KATSOULI</t>
+          <t>JAMES QUENTIN BURNS</t>
         </is>
       </c>
       <c r="C3532" t="n">
@@ -46354,7 +46354,7 @@
       </c>
       <c r="B3533" t="inlineStr">
         <is>
-          <t>STIPE GASPIC</t>
+          <t>CONRAD KONITZER, ANTONIO TORRADO MARTINEZ</t>
         </is>
       </c>
       <c r="C3533" t="n">
@@ -46367,7 +46367,7 @@
       </c>
       <c r="B3534" t="inlineStr">
         <is>
-          <t>NIKOLE BARNES, TED MCDONOUGH</t>
+          <t>SANDRA LULIC</t>
         </is>
       </c>
       <c r="C3534" t="n">
@@ -46380,7 +46380,7 @@
       </c>
       <c r="B3535" t="inlineStr">
         <is>
-          <t>OTTO HENRY</t>
+          <t>CHRIS BOBOTAS</t>
         </is>
       </c>
       <c r="C3535" t="n">
@@ -46393,7 +46393,7 @@
       </c>
       <c r="B3536" t="inlineStr">
         <is>
-          <t>ANTON MESSERITSCH</t>
+          <t>KARL MARTIN RAMMO</t>
         </is>
       </c>
       <c r="C3536" t="n">
@@ -46406,7 +46406,7 @@
       </c>
       <c r="B3537" t="inlineStr">
         <is>
-          <t>HENRIQUE HADDAD, ISABEL SWAN</t>
+          <t>IAKOVOS CHRISTOFIDIS</t>
         </is>
       </c>
       <c r="C3537" t="n">
@@ -46419,7 +46419,7 @@
       </c>
       <c r="B3538" t="inlineStr">
         <is>
-          <t>KAARLE TAPPER</t>
+          <t>RADVILAS JANULIONIS</t>
         </is>
       </c>
       <c r="C3538" t="n">
@@ -46432,7 +46432,7 @@
       </c>
       <c r="B3539" t="inlineStr">
         <is>
-          <t>YU CHEN</t>
+          <t>LEONARD COLLADO</t>
         </is>
       </c>
       <c r="C3539" t="n">
@@ -46445,7 +46445,7 @@
       </c>
       <c r="B3540" t="inlineStr">
         <is>
-          <t>HU XIAOYU, SHAN MENGYUAN</t>
+          <t>JANA GERMANI, GIORGIA BERTUZZI</t>
         </is>
       </c>
       <c r="C3540" t="n">
@@ -46458,7 +46458,7 @@
       </c>
       <c r="B3541" t="inlineStr">
         <is>
-          <t>MARIA JOSE CUCALON, JONATHAN MARTINETTI</t>
+          <t>ANNE MARIE RINDOM</t>
         </is>
       </c>
       <c r="C3541" t="n">
@@ -46471,7 +46471,7 @@
       </c>
       <c r="B3542" t="inlineStr">
         <is>
-          <t>RINA  NIIJIMA</t>
+          <t>BERNAT TOMAS</t>
         </is>
       </c>
       <c r="C3542" t="n">
@@ -46484,7 +46484,7 @@
       </c>
       <c r="B3543" t="inlineStr">
         <is>
-          <t>FACUNDO OLEZZA</t>
+          <t>HERMIONIE GHICAS</t>
         </is>
       </c>
       <c r="C3543" t="n">
@@ -46497,7 +46497,7 @@
       </c>
       <c r="B3544" t="inlineStr">
         <is>
-          <t>UFFE TOMASGAARD</t>
+          <t>POULIQUEN YUN</t>
         </is>
       </c>
       <c r="C3544" t="n">
@@ -46510,7 +46510,7 @@
       </c>
       <c r="B3545" t="inlineStr">
         <is>
-          <t>PERNELLE MICHON</t>
+          <t>PIERRE  LE COQ</t>
         </is>
       </c>
       <c r="C3545" t="n">
@@ -46523,7 +46523,7 @@
       </c>
       <c r="B3546" t="inlineStr">
         <is>
-          <t>SOPHIA  MEYER</t>
+          <t>JAMES GRUMMETT, RHOS HAWES</t>
         </is>
       </c>
       <c r="C3546" t="n">
@@ -46536,7 +46536,7 @@
       </c>
       <c r="B3547" t="inlineStr">
         <is>
-          <t>ADA TAN</t>
+          <t>JULIAN TAYLOR</t>
         </is>
       </c>
       <c r="C3547" t="n">
@@ -46549,7 +46549,7 @@
       </c>
       <c r="B3548" t="inlineStr">
         <is>
-          <t>HAMISH GILSENAN</t>
+          <t>JOSEPH JONATHAN PEN WESTON</t>
         </is>
       </c>
       <c r="C3548" t="n">
@@ -46562,7 +46562,7 @@
       </c>
       <c r="B3549" t="inlineStr">
         <is>
-          <t>ALFONSO FERNANDEZ</t>
+          <t>WANG YINGQIAN, XIAOYA SU</t>
         </is>
       </c>
       <c r="C3549" t="n">
@@ -46575,7 +46575,7 @@
       </c>
       <c r="B3550" t="inlineStr">
         <is>
-          <t>ZAN LUKA ZELKO</t>
+          <t>CHARLIE LEIGH, RYAN ORR</t>
         </is>
       </c>
       <c r="C3550" t="n">
@@ -46588,7 +46588,7 @@
       </c>
       <c r="B3551" t="inlineStr">
         <is>
-          <t>ANIL GARNIER</t>
+          <t>NICO PARLIER</t>
         </is>
       </c>
       <c r="C3551" t="n">
@@ -46601,7 +46601,7 @@
       </c>
       <c r="B3552" t="inlineStr">
         <is>
-          <t>ENRICHETTA BETTINI FLEITAS</t>
+          <t>FERRUCCIO ARVEDI</t>
         </is>
       </c>
       <c r="C3552" t="n">
@@ -46614,7 +46614,7 @@
       </c>
       <c r="B3553" t="inlineStr">
         <is>
-          <t>QIBIN HUANG</t>
+          <t>TYTUS BUTOWSKI, BORYS PODUMIS</t>
         </is>
       </c>
       <c r="C3553" t="n">
@@ -46627,7 +46627,7 @@
       </c>
       <c r="B3554" t="inlineStr">
         <is>
-          <t>JOSEPHINE P W FREDERIKSEN, LAURA STEENSTRUP ZEEBERG</t>
+          <t>LUCA VALENTINO</t>
         </is>
       </c>
       <c r="C3554" t="n">
@@ -46640,7 +46640,7 @@
       </c>
       <c r="B3555" t="inlineStr">
         <is>
-          <t>KAZUMASA SEGAWA</t>
+          <t>CANNELLE OPSTAELE</t>
         </is>
       </c>
       <c r="C3555" t="n">
@@ -46653,7 +46653,7 @@
       </c>
       <c r="B3556" t="inlineStr">
         <is>
-          <t>JOSH MORGAN</t>
+          <t>CAMILLE LECOINTRE, JEREMIE MION</t>
         </is>
       </c>
       <c r="C3556" t="n">
@@ -46666,7 +46666,7 @@
       </c>
       <c r="B3557" t="inlineStr">
         <is>
-          <t>JOSEFIN OLSSON</t>
+          <t>OMER VERED VILENCHIK</t>
         </is>
       </c>
       <c r="C3557" t="n">
@@ -46679,7 +46679,7 @@
       </c>
       <c r="B3558" t="inlineStr">
         <is>
-          <t>NOCETI KLEPACKA ZOFIA</t>
+          <t>JAGO HUERCANOS MACHIMBARRENA</t>
         </is>
       </c>
       <c r="C3558" t="n">
@@ -46692,7 +46692,7 @@
       </c>
       <c r="B3559" t="inlineStr">
         <is>
-          <t>BENJAMIN AGANOVIE</t>
+          <t>LUC CHEVRIER</t>
         </is>
       </c>
       <c r="C3559" t="n">
@@ -46705,7 +46705,7 @@
       </c>
       <c r="B3560" t="inlineStr">
         <is>
-          <t>CAMPBELL STANTON, WILL SHAPLAND</t>
+          <t>TERUAKI SHIMAKURA, KAMISONODA SHINTARO SEIJI</t>
         </is>
       </c>
       <c r="C3560" t="n">
@@ -46718,7 +46718,7 @@
       </c>
       <c r="B3561" t="inlineStr">
         <is>
-          <t>ROSA DONNER, NIKLAS HABERL</t>
+          <t>NICO NAUJOCK</t>
         </is>
       </c>
       <c r="C3561" t="n">
@@ -46731,7 +46731,7 @@
       </c>
       <c r="B3562" t="inlineStr">
         <is>
-          <t>GIAN STRAGIOTTI</t>
+          <t>STEFAN ELLIOTT SHIRCORE</t>
         </is>
       </c>
       <c r="C3562" t="n">
@@ -46744,7 +46744,7 @@
       </c>
       <c r="B3563" t="inlineStr">
         <is>
-          <t>FINN LYNCH</t>
+          <t>INGA-MARIE HOFMANN, CATHERINE BARTELHEIMER</t>
         </is>
       </c>
       <c r="C3563" t="n">
@@ -46757,7 +46757,7 @@
       </c>
       <c r="B3564" t="inlineStr">
         <is>
-          <t>YUMIKO TOMBE</t>
+          <t>CHRIS THORPE</t>
         </is>
       </c>
       <c r="C3564" t="n">
@@ -46770,7 +46770,7 @@
       </c>
       <c r="B3565" t="inlineStr">
         <is>
-          <t>ELLIOTT WELLS BILLY, VENNIS-OZANNE</t>
+          <t>ALEJANDRO CLIMENT</t>
         </is>
       </c>
       <c r="C3565" t="n">

</xml_diff>